<commit_message>
Implemented MoECapacityCalcService to conduct means of escape capacity calcs.
Refactored HorizontalEscapeCapacityService such that ExitCapacityStruct logic is handled by ExitCapacityStructService.

Added names to CapacityStructs to make it easier to determine what is being tracked.

Extracted Discounting and Capping logic to a dedicated service such that it may be shared between Horizontal and MoE Capacity Calc Services.

Updated Tests to reflect above - more integration tests required for MoECapacityCalc
</commit_message>
<xml_diff>
--- a/ExcelTestData/AreaHMoECapacityTest2.xlsx
+++ b/ExcelTestData/AreaHMoECapacityTest2.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="91">
   <si>
     <t xml:space="preserve">Stair capacity factors</t>
   </si>
@@ -377,6 +377,21 @@
   </si>
   <si>
     <t xml:space="preserve">Merging flow capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StoreyExit 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FinalExit 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If Area is on upper floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacity = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If Area is on final exit level of all stairs</t>
   </si>
 </sst>
 </file>
@@ -506,7 +521,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -569,10 +584,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -702,9 +713,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>64440</xdr:colOff>
+      <xdr:colOff>64080</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>14400</xdr:rowOff>
+      <xdr:rowOff>14040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -717,8 +728,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15707880" y="2081520"/>
-          <a:ext cx="3156480" cy="1009440"/>
+          <a:off x="16114680" y="2081520"/>
+          <a:ext cx="3157560" cy="1009080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -744,7 +755,7 @@
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.17"/>
@@ -757,7 +768,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="31.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="27.46"/>
@@ -2057,33 +2068,33 @@
       <c r="B40" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="16" t="n">
+      <c r="C40" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;C$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;C$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="D40" s="16" t="n">
+      <c r="D40" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;D$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;D$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="E40" s="16" t="n">
+      <c r="E40" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;E$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;E$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>528</v>
       </c>
-      <c r="M40" s="17" t="s">
+      <c r="M40" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="N40" s="18" t="n">
+      <c r="N40" s="17" t="n">
         <v>3300</v>
       </c>
-      <c r="O40" s="18" t="n">
+      <c r="O40" s="17" t="n">
         <f aca="false">N40/6</f>
         <v>550</v>
       </c>
-      <c r="P40" s="18" t="n">
+      <c r="P40" s="17" t="n">
         <f aca="false">N40/10</f>
         <v>330</v>
       </c>
-      <c r="Q40" s="19" t="n">
+      <c r="Q40" s="18" t="n">
         <f aca="false">N40/SUM(C45:E45)</f>
         <v>3.85514018691589</v>
       </c>
@@ -2092,33 +2103,33 @@
       <c r="B41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="16" t="n">
+      <c r="C41" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;C$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;C$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="D41" s="16" t="n">
+      <c r="D41" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;D$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;D$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="E41" s="16" t="n">
+      <c r="E41" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;E$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;E$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>528</v>
       </c>
-      <c r="M41" s="17" t="s">
+      <c r="M41" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="N41" s="18" t="n">
+      <c r="N41" s="17" t="n">
         <v>4680</v>
       </c>
-      <c r="O41" s="18" t="n">
+      <c r="O41" s="17" t="n">
         <f aca="false">N41/6</f>
         <v>780</v>
       </c>
-      <c r="P41" s="18" t="n">
+      <c r="P41" s="17" t="n">
         <f aca="false">N41/10</f>
         <v>468</v>
       </c>
-      <c r="Q41" s="19" t="n">
+      <c r="Q41" s="18" t="n">
         <f aca="false">N41/SUM(C44:E44)</f>
         <v>5.46728971962617</v>
       </c>
@@ -2127,33 +2138,33 @@
       <c r="B42" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C42" s="16" t="n">
+      <c r="C42" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;C$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;C$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="D42" s="16" t="n">
+      <c r="D42" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;D$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;D$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="E42" s="16" t="n">
+      <c r="E42" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;E$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;E$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>528</v>
       </c>
-      <c r="M42" s="17" t="n">
+      <c r="M42" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="N42" s="18" t="n">
+      <c r="N42" s="17" t="n">
         <v>8060</v>
       </c>
-      <c r="O42" s="18" t="n">
+      <c r="O42" s="17" t="n">
         <f aca="false">N42/6</f>
         <v>1343.33333333333</v>
       </c>
-      <c r="P42" s="18" t="n">
+      <c r="P42" s="17" t="n">
         <f aca="false">N42/10</f>
         <v>806</v>
       </c>
-      <c r="Q42" s="19" t="n">
+      <c r="Q42" s="18" t="n">
         <f aca="false">N42/SUM(C43:E43)</f>
         <v>5.82369942196532</v>
       </c>
@@ -2162,33 +2173,33 @@
       <c r="B43" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="16" t="n">
+      <c r="C43" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;C$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;C$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="D43" s="16" t="n">
+      <c r="D43" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;D$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;D$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="E43" s="16" t="n">
+      <c r="E43" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;E$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;E$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>528</v>
       </c>
-      <c r="M43" s="17" t="n">
+      <c r="M43" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="N43" s="18" t="n">
+      <c r="N43" s="17" t="n">
         <v>8060</v>
       </c>
-      <c r="O43" s="18" t="n">
+      <c r="O43" s="17" t="n">
         <f aca="false">N43/6</f>
         <v>1343.33333333333</v>
       </c>
-      <c r="P43" s="18" t="n">
+      <c r="P43" s="17" t="n">
         <f aca="false">N43/10</f>
         <v>806</v>
       </c>
-      <c r="Q43" s="19" t="n">
+      <c r="Q43" s="18" t="n">
         <f aca="false">N43/SUM(C42:E42)</f>
         <v>5.82369942196532</v>
       </c>
@@ -2197,32 +2208,32 @@
       <c r="B44" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C44" s="16" t="n">
+      <c r="C44" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;C$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;C$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="D44" s="16" t="n">
+      <c r="D44" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;D$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;D$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="M44" s="17" t="n">
+      <c r="M44" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="N44" s="18" t="n">
+      <c r="N44" s="17" t="n">
         <v>8060</v>
       </c>
-      <c r="O44" s="18" t="n">
+      <c r="O44" s="17" t="n">
         <f aca="false">N44/6</f>
         <v>1343.33333333333</v>
       </c>
-      <c r="P44" s="18" t="n">
+      <c r="P44" s="17" t="n">
         <f aca="false">N44/10</f>
         <v>806</v>
       </c>
-      <c r="Q44" s="19" t="n">
+      <c r="Q44" s="18" t="n">
         <f aca="false">N44/SUM(C41:E41)</f>
         <v>5.82369942196532</v>
       </c>
@@ -2231,55 +2242,55 @@
       <c r="B45" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C45" s="16" t="n">
+      <c r="C45" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;C$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;C$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="D45" s="16" t="n">
+      <c r="D45" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;D$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;D$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="E45" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="M45" s="17" t="n">
+      <c r="M45" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="N45" s="18" t="n">
+      <c r="N45" s="17" t="n">
         <v>7960</v>
       </c>
-      <c r="O45" s="18" t="n">
+      <c r="O45" s="17" t="n">
         <f aca="false">N45/6</f>
         <v>1326.66666666667</v>
       </c>
-      <c r="P45" s="18" t="n">
+      <c r="P45" s="17" t="n">
         <f aca="false">N45/10</f>
         <v>796</v>
       </c>
-      <c r="Q45" s="19" t="n">
+      <c r="Q45" s="18" t="n">
         <f aca="false">N45/SUM(C40:E40)</f>
         <v>5.7514450867052</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="M46" s="17" t="s">
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="M46" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="N46" s="18" t="n">
+      <c r="N46" s="17" t="n">
         <v>7380</v>
       </c>
-      <c r="O46" s="18" t="n">
+      <c r="O46" s="17" t="n">
         <f aca="false">N46/6</f>
         <v>1230</v>
       </c>
-      <c r="P46" s="18" t="n">
+      <c r="P46" s="17" t="n">
         <f aca="false">N46/10</f>
         <v>738</v>
       </c>
-      <c r="Q46" s="19" t="n">
+      <c r="Q46" s="18" t="n">
         <f aca="false">N46/SUM(C39:E39)</f>
         <v>4.07284768211921</v>
       </c>
@@ -2301,33 +2312,33 @@
         <v>2716</v>
       </c>
       <c r="G47" s="1"/>
-      <c r="M47" s="17" t="s">
+      <c r="M47" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="N47" s="18" t="n">
+      <c r="N47" s="17" t="n">
         <f aca="false">SUM(N40:N46)</f>
         <v>47500</v>
       </c>
-      <c r="O47" s="18" t="n">
+      <c r="O47" s="17" t="n">
         <f aca="false">SUM(O40:O46)</f>
         <v>7916.66666666667</v>
       </c>
-      <c r="P47" s="18" t="n">
+      <c r="P47" s="17" t="n">
         <f aca="false">SUM(P40:P46)</f>
         <v>4750</v>
       </c>
-      <c r="Q47" s="19" t="e">
+      <c r="Q47" s="18" t="e">
         <f aca="false">N47/SUM(C52:E52)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="20" t="n">
+      <c r="C48" s="19" t="n">
         <f aca="false">SUM(C47:E47)</f>
         <v>9060</v>
       </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2351,12 +2362,12 @@
   <dimension ref="B1:R45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.82"/>
@@ -2369,7 +2380,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.91"/>
   </cols>
   <sheetData>
@@ -2393,14 +2404,14 @@
         <v>75</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="H2" s="0" t="n">
         <f aca="false">200*(G2/1000)+50*((G2/1000)-0.3)*(F2-1)</f>
-        <v>645</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2413,18 +2424,18 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="19"/>
-      <c r="C5" s="21" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
       <c r="M5" s="1" t="s">
         <v>78</v>
       </c>
@@ -2436,41 +2447,41 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="23" t="n">
+      <c r="C6" s="22" t="n">
         <v>1000</v>
       </c>
-      <c r="D6" s="23" t="n">
+      <c r="D6" s="22" t="n">
         <f aca="false">C6+100</f>
         <v>1100</v>
       </c>
-      <c r="E6" s="23" t="n">
+      <c r="E6" s="22" t="n">
         <f aca="false">D6+100</f>
         <v>1200</v>
       </c>
-      <c r="F6" s="23" t="n">
+      <c r="F6" s="22" t="n">
         <f aca="false">E6+100</f>
         <v>1300</v>
       </c>
-      <c r="G6" s="23" t="n">
+      <c r="G6" s="22" t="n">
         <f aca="false">F6+100</f>
         <v>1400</v>
       </c>
-      <c r="H6" s="23" t="n">
+      <c r="H6" s="22" t="n">
         <f aca="false">G6+100</f>
         <v>1500</v>
       </c>
-      <c r="I6" s="23" t="n">
+      <c r="I6" s="22" t="n">
         <f aca="false">H6+100</f>
         <v>1600</v>
       </c>
-      <c r="J6" s="23" t="n">
+      <c r="J6" s="22" t="n">
         <f aca="false">I6+100</f>
         <v>1700</v>
       </c>
-      <c r="K6" s="23" t="n">
+      <c r="K6" s="22" t="n">
         <f aca="false">J6+100</f>
         <v>1800</v>
       </c>
@@ -2485,34 +2496,34 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="22" t="n">
+      <c r="B7" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="24" t="n">
+      <c r="C7" s="23" t="n">
         <v>150</v>
       </c>
-      <c r="D7" s="24" t="n">
+      <c r="D7" s="23" t="n">
         <v>220</v>
       </c>
-      <c r="E7" s="24" t="n">
+      <c r="E7" s="23" t="n">
         <v>240</v>
       </c>
-      <c r="F7" s="24" t="n">
+      <c r="F7" s="23" t="n">
         <v>260</v>
       </c>
-      <c r="G7" s="24" t="n">
+      <c r="G7" s="23" t="n">
         <v>280</v>
       </c>
-      <c r="H7" s="24" t="n">
+      <c r="H7" s="23" t="n">
         <v>300</v>
       </c>
-      <c r="I7" s="24" t="n">
+      <c r="I7" s="23" t="n">
         <v>320</v>
       </c>
-      <c r="J7" s="24" t="n">
+      <c r="J7" s="23" t="n">
         <v>340</v>
       </c>
-      <c r="K7" s="24" t="n">
+      <c r="K7" s="23" t="n">
         <v>360</v>
       </c>
       <c r="M7" s="1" t="n">
@@ -2526,34 +2537,34 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="22" t="n">
+      <c r="B8" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="24" t="n">
+      <c r="C8" s="23" t="n">
         <v>190</v>
       </c>
-      <c r="D8" s="24" t="n">
+      <c r="D8" s="23" t="n">
         <v>260</v>
       </c>
-      <c r="E8" s="24" t="n">
+      <c r="E8" s="23" t="n">
         <v>285</v>
       </c>
-      <c r="F8" s="24" t="n">
+      <c r="F8" s="23" t="n">
         <v>310</v>
       </c>
-      <c r="G8" s="24" t="n">
+      <c r="G8" s="23" t="n">
         <v>335</v>
       </c>
-      <c r="H8" s="24" t="n">
+      <c r="H8" s="23" t="n">
         <v>360</v>
       </c>
-      <c r="I8" s="24" t="n">
+      <c r="I8" s="23" t="n">
         <v>385</v>
       </c>
-      <c r="J8" s="24" t="n">
+      <c r="J8" s="23" t="n">
         <v>410</v>
       </c>
-      <c r="K8" s="24" t="n">
+      <c r="K8" s="23" t="n">
         <v>435</v>
       </c>
       <c r="M8" s="1" t="n">
@@ -2567,37 +2578,37 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="22" t="n">
+      <c r="B9" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="24" t="n">
+      <c r="C9" s="23" t="n">
         <v>230</v>
       </c>
-      <c r="D9" s="24" t="n">
+      <c r="D9" s="23" t="n">
         <v>300</v>
       </c>
-      <c r="E9" s="24" t="n">
+      <c r="E9" s="23" t="n">
         <v>330</v>
       </c>
-      <c r="F9" s="24" t="n">
+      <c r="F9" s="23" t="n">
         <v>360</v>
       </c>
-      <c r="G9" s="24" t="n">
+      <c r="G9" s="23" t="n">
         <v>390</v>
       </c>
-      <c r="H9" s="24" t="n">
+      <c r="H9" s="23" t="n">
         <v>420</v>
       </c>
-      <c r="I9" s="24" t="n">
+      <c r="I9" s="23" t="n">
         <v>450</v>
       </c>
-      <c r="J9" s="24" t="n">
+      <c r="J9" s="23" t="n">
         <v>480</v>
       </c>
-      <c r="K9" s="24" t="n">
+      <c r="K9" s="23" t="n">
         <v>510</v>
       </c>
-      <c r="M9" s="25" t="s">
+      <c r="M9" s="24" t="s">
         <v>81</v>
       </c>
       <c r="N9" s="3" t="s">
@@ -2608,228 +2619,228 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="22" t="n">
+      <c r="B10" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="24" t="n">
+      <c r="C10" s="23" t="n">
         <v>270</v>
       </c>
-      <c r="D10" s="24" t="n">
+      <c r="D10" s="23" t="n">
         <v>340</v>
       </c>
-      <c r="E10" s="24" t="n">
+      <c r="E10" s="23" t="n">
         <v>375</v>
       </c>
-      <c r="F10" s="24" t="n">
+      <c r="F10" s="23" t="n">
         <v>410</v>
       </c>
-      <c r="G10" s="24" t="n">
+      <c r="G10" s="23" t="n">
         <v>445</v>
       </c>
-      <c r="H10" s="24" t="n">
+      <c r="H10" s="23" t="n">
         <v>480</v>
       </c>
-      <c r="I10" s="24" t="n">
+      <c r="I10" s="23" t="n">
         <v>515</v>
       </c>
-      <c r="J10" s="24" t="n">
+      <c r="J10" s="23" t="n">
         <v>550</v>
       </c>
-      <c r="K10" s="24" t="n">
+      <c r="K10" s="23" t="n">
         <v>585</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="22" t="n">
+      <c r="B11" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="24" t="n">
+      <c r="C11" s="23" t="n">
         <v>310</v>
       </c>
-      <c r="D11" s="24" t="n">
+      <c r="D11" s="23" t="n">
         <v>380</v>
       </c>
-      <c r="E11" s="24" t="n">
+      <c r="E11" s="23" t="n">
         <v>420</v>
       </c>
-      <c r="F11" s="24" t="n">
+      <c r="F11" s="23" t="n">
         <v>460</v>
       </c>
-      <c r="G11" s="24" t="n">
+      <c r="G11" s="23" t="n">
         <v>500</v>
       </c>
-      <c r="H11" s="24" t="n">
+      <c r="H11" s="23" t="n">
         <v>540</v>
       </c>
-      <c r="I11" s="24" t="n">
+      <c r="I11" s="23" t="n">
         <v>580</v>
       </c>
-      <c r="J11" s="24" t="n">
+      <c r="J11" s="23" t="n">
         <v>620</v>
       </c>
-      <c r="K11" s="24" t="n">
+      <c r="K11" s="23" t="n">
         <v>660</v>
       </c>
       <c r="L11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="22" t="n">
+      <c r="B12" s="21" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="24" t="n">
+      <c r="C12" s="23" t="n">
         <v>350</v>
       </c>
-      <c r="D12" s="24" t="n">
+      <c r="D12" s="23" t="n">
         <v>420</v>
       </c>
-      <c r="E12" s="24" t="n">
+      <c r="E12" s="23" t="n">
         <v>465</v>
       </c>
-      <c r="F12" s="24" t="n">
+      <c r="F12" s="23" t="n">
         <v>510</v>
       </c>
-      <c r="G12" s="24" t="n">
+      <c r="G12" s="23" t="n">
         <v>555</v>
       </c>
-      <c r="H12" s="24" t="n">
+      <c r="H12" s="23" t="n">
         <v>600</v>
       </c>
-      <c r="I12" s="24" t="n">
+      <c r="I12" s="23" t="n">
         <v>645</v>
       </c>
-      <c r="J12" s="24" t="n">
+      <c r="J12" s="23" t="n">
         <v>690</v>
       </c>
-      <c r="K12" s="24" t="n">
+      <c r="K12" s="23" t="n">
         <v>735</v>
       </c>
       <c r="L12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="22" t="n">
+      <c r="B13" s="21" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="24" t="n">
+      <c r="C13" s="23" t="n">
         <v>390</v>
       </c>
-      <c r="D13" s="24" t="n">
+      <c r="D13" s="23" t="n">
         <v>460</v>
       </c>
-      <c r="E13" s="24" t="n">
+      <c r="E13" s="23" t="n">
         <v>510</v>
       </c>
-      <c r="F13" s="24" t="n">
+      <c r="F13" s="23" t="n">
         <v>560</v>
       </c>
-      <c r="G13" s="24" t="n">
+      <c r="G13" s="23" t="n">
         <v>610</v>
       </c>
-      <c r="H13" s="24" t="n">
+      <c r="H13" s="23" t="n">
         <v>660</v>
       </c>
-      <c r="I13" s="24" t="n">
+      <c r="I13" s="23" t="n">
         <v>710</v>
       </c>
-      <c r="J13" s="24" t="n">
+      <c r="J13" s="23" t="n">
         <v>760</v>
       </c>
-      <c r="K13" s="24" t="n">
+      <c r="K13" s="23" t="n">
         <v>810</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="22" t="n">
+      <c r="B14" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="24" t="n">
+      <c r="C14" s="23" t="n">
         <v>430</v>
       </c>
-      <c r="D14" s="24" t="n">
+      <c r="D14" s="23" t="n">
         <v>500</v>
       </c>
-      <c r="E14" s="24" t="n">
+      <c r="E14" s="23" t="n">
         <v>555</v>
       </c>
-      <c r="F14" s="24" t="n">
+      <c r="F14" s="23" t="n">
         <v>610</v>
       </c>
-      <c r="G14" s="24" t="n">
+      <c r="G14" s="23" t="n">
         <v>665</v>
       </c>
-      <c r="H14" s="24" t="n">
+      <c r="H14" s="23" t="n">
         <v>720</v>
       </c>
-      <c r="I14" s="24" t="n">
+      <c r="I14" s="23" t="n">
         <v>775</v>
       </c>
-      <c r="J14" s="24" t="n">
+      <c r="J14" s="23" t="n">
         <v>830</v>
       </c>
-      <c r="K14" s="24" t="n">
+      <c r="K14" s="23" t="n">
         <v>885</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="22" t="n">
+      <c r="B15" s="21" t="n">
         <v>9</v>
       </c>
-      <c r="C15" s="24" t="n">
+      <c r="C15" s="23" t="n">
         <v>470</v>
       </c>
-      <c r="D15" s="24" t="n">
+      <c r="D15" s="23" t="n">
         <v>540</v>
       </c>
-      <c r="E15" s="24" t="n">
+      <c r="E15" s="23" t="n">
         <v>600</v>
       </c>
-      <c r="F15" s="24" t="n">
+      <c r="F15" s="23" t="n">
         <v>660</v>
       </c>
-      <c r="G15" s="24" t="n">
+      <c r="G15" s="23" t="n">
         <v>720</v>
       </c>
-      <c r="H15" s="24" t="n">
+      <c r="H15" s="23" t="n">
         <v>780</v>
       </c>
-      <c r="I15" s="24" t="n">
+      <c r="I15" s="23" t="n">
         <v>840</v>
       </c>
-      <c r="J15" s="24" t="n">
+      <c r="J15" s="23" t="n">
         <v>900</v>
       </c>
-      <c r="K15" s="24" t="n">
+      <c r="K15" s="23" t="n">
         <v>960</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="22" t="n">
+      <c r="B16" s="21" t="n">
         <v>10</v>
       </c>
-      <c r="C16" s="24" t="n">
+      <c r="C16" s="23" t="n">
         <v>510</v>
       </c>
-      <c r="D16" s="24" t="n">
+      <c r="D16" s="23" t="n">
         <v>580</v>
       </c>
-      <c r="E16" s="24" t="n">
+      <c r="E16" s="23" t="n">
         <v>645</v>
       </c>
-      <c r="F16" s="24" t="n">
+      <c r="F16" s="23" t="n">
         <v>710</v>
       </c>
-      <c r="G16" s="24" t="n">
+      <c r="G16" s="23" t="n">
         <v>775</v>
       </c>
-      <c r="H16" s="24" t="n">
+      <c r="H16" s="23" t="n">
         <v>840</v>
       </c>
-      <c r="I16" s="24" t="n">
+      <c r="I16" s="23" t="n">
         <v>905</v>
       </c>
-      <c r="J16" s="24" t="n">
+      <c r="J16" s="23" t="n">
         <v>970</v>
       </c>
-      <c r="K16" s="24" t="n">
+      <c r="K16" s="23" t="n">
         <v>1035</v>
       </c>
     </row>
@@ -2837,42 +2848,42 @@
       <c r="B17" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="26" t="s">
+      <c r="H19" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="I19" s="26" t="s">
+      <c r="I19" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="J19" s="26" t="s">
+      <c r="J19" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="K19" s="26"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="26" t="s">
+      <c r="K19" s="25"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="N19" s="26" t="s">
+      <c r="N19" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="O19" s="26" t="s">
+      <c r="O19" s="25" t="s">
         <v>32</v>
       </c>
       <c r="P19" s="1" t="s">
@@ -2885,7 +2896,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>36</v>
       </c>
@@ -2893,52 +2904,48 @@
         <v>37</v>
       </c>
       <c r="D20" s="6" t="n">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F20" s="8" t="n">
-        <f aca="false">200*(D20/1000)+50*((D20/1000)-0.3)*(E20-1)</f>
-        <v>420</v>
+        <v>230</v>
       </c>
       <c r="G20" s="5" t="n">
         <f aca="false">ROUNDDOWN(F20/E20,0)</f>
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>38</v>
       </c>
       <c r="I20" s="0" t="n">
-        <v>850</v>
+        <v>1050</v>
       </c>
       <c r="J20" s="5" t="n">
         <f aca="false" t="array" ref="J20:J20">_xlfn.IFS(AND($I20&gt;=$M$6,$I20&lt;$M$7),$N$6,AND($I20&gt;=$M$7,$I20&lt;$M$8),$N$7,$I20&gt;=$M$8,$N$8+($I20-$M$8)/5)</f>
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="K20" s="5"/>
       <c r="M20" s="9" t="n">
-        <v>1500</v>
+        <f aca="false">1050+0.5*1050</f>
+        <v>1575</v>
       </c>
       <c r="N20" s="5" t="n">
         <f aca="false" t="array" ref="N20:N20">_xlfn.IFS(AND($M20&gt;=$M$6,$M20&lt;$M$7),$N$6,AND($M20&gt;=$M$7,$M20&lt;$M$8),$N$7,$M20&gt;=$M$8,$N$8+($M20-$M$8)/5)</f>
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="O20" s="0" t="n">
         <f aca="false">ROUNDDOWN(N20/E20,0)</f>
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="P20" s="0" t="n">
         <f aca="false">MIN((ROUNDDOWN(N20,0)),ROUNDDOWN(((((M20)/1000)*80)-(60*(D20/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q20" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P20/2,0)</f>
-        <v>67</v>
+        <v>165</v>
       </c>
       <c r="R20" s="11"/>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
         <v>36</v>
       </c>
@@ -2949,48 +2956,45 @@
         <v>1100</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F21" s="8" t="n">
         <f aca="false">200*(D21/1000)+50*((D21/1000)-0.3)*(E21-1)</f>
-        <v>420</v>
+        <v>300</v>
       </c>
       <c r="G21" s="5" t="n">
         <f aca="false">ROUNDDOWN(F21/E21,0)</f>
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>38</v>
       </c>
       <c r="I21" s="0" t="n">
-        <v>850</v>
+        <v>1050</v>
       </c>
       <c r="J21" s="5" t="n">
         <f aca="false" t="array" ref="J21:J21">_xlfn.IFS(AND($I21&gt;=$M$6,$I21&lt;$M$7),$N$6,AND($I21&gt;=$M$7,$I21&lt;$M$8),$N$7,$I21&gt;=$M$8,$N$8+($I21-$M$8)/5)</f>
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="K21" s="5"/>
       <c r="M21" s="9" t="n">
-        <v>1500</v>
+        <f aca="false">1050+0.5*1050</f>
+        <v>1575</v>
       </c>
       <c r="N21" s="5" t="n">
         <f aca="false" t="array" ref="N21:N21">_xlfn.IFS(AND($M21&gt;=$M$6,$M21&lt;$M$7),$N$6,AND($M21&gt;=$M$7,$M21&lt;$M$8),$N$7,$M21&gt;=$M$8,$N$8+($M21-$M$8)/5)</f>
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="O21" s="0" t="n">
         <f aca="false">ROUNDDOWN(N21/E21,0)</f>
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="P21" s="0" t="n">
         <f aca="false">MIN((ROUNDDOWN(N21,0)),ROUNDDOWN((((M21/1000)*80)-(60*(D21/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q21" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P21/2,0)</f>
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>36</v>
       </c>
@@ -2998,52 +3002,48 @@
         <v>41</v>
       </c>
       <c r="D22" s="6" t="n">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F22" s="8" t="n">
-        <f aca="false">200*(D22/1000)+50*((D22/1000)-0.3)*(E22-1)</f>
-        <v>420</v>
+        <v>230</v>
       </c>
       <c r="G22" s="5" t="n">
         <f aca="false">ROUNDDOWN(F22/E22,0)</f>
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>38</v>
       </c>
       <c r="I22" s="0" t="n">
-        <v>850</v>
+        <v>1050</v>
       </c>
       <c r="J22" s="5" t="n">
         <f aca="false" t="array" ref="J22:J22">_xlfn.IFS(AND($I22&gt;=$M$6,$I22&lt;$M$7),$N$6,AND($I22&gt;=$M$7,$I22&lt;$M$8),$N$7,$I22&gt;=$M$8,$N$8+($I22-$M$8)/5)</f>
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="K22" s="5"/>
       <c r="M22" s="9" t="n">
-        <v>1500</v>
+        <f aca="false">1050+0.5*1050</f>
+        <v>1575</v>
       </c>
       <c r="N22" s="5" t="n">
         <f aca="false" t="array" ref="N22:N22">_xlfn.IFS(AND($M22&gt;=$M$6,$M22&lt;$M$7),$N$6,AND($M22&gt;=$M$7,$M22&lt;$M$8),$N$7,$M22&gt;=$M$8,$N$8+($M22-$M$8)/5)</f>
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="O22" s="0" t="n">
         <f aca="false">ROUNDDOWN(N22/E22,0)</f>
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="P22" s="0" t="n">
         <f aca="false">MIN((ROUNDDOWN(N22,0)),ROUNDDOWN((((M22/1000)*80)-(60*(D22/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q22" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P22/2,0)</f>
-        <v>67</v>
+        <v>165</v>
       </c>
       <c r="R22" s="11"/>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
         <v>36</v>
       </c>
@@ -3054,469 +3054,178 @@
         <v>1100</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F23" s="8" t="n">
         <f aca="false">200*(D23/1000)+50*((D23/1000)-0.3)*(E23-1)</f>
-        <v>420</v>
+        <v>300</v>
       </c>
       <c r="G23" s="5" t="n">
         <f aca="false">ROUNDDOWN(F23/E23,0)</f>
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>38</v>
       </c>
       <c r="I23" s="0" t="n">
-        <v>850</v>
+        <v>1050</v>
       </c>
       <c r="J23" s="5" t="n">
         <f aca="false" t="array" ref="J23:J23">_xlfn.IFS(AND($I23&gt;=$M$6,$I23&lt;$M$7),$N$6,AND($I23&gt;=$M$7,$I23&lt;$M$8),$N$7,$I23&gt;=$M$8,$N$8+($I23-$M$8)/5)</f>
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="K23" s="5"/>
       <c r="M23" s="9" t="n">
-        <v>1500</v>
+        <f aca="false">1050+0.5*1050</f>
+        <v>1575</v>
       </c>
       <c r="N23" s="5" t="n">
         <f aca="false" t="array" ref="N23:N23">_xlfn.IFS(AND($M23&gt;=$M$6,$M23&lt;$M$7),$N$6,AND($M23&gt;=$M$7,$M23&lt;$M$8),$N$7,$M23&gt;=$M$8,$N$8+($M23-$M$8)/5)</f>
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="O23" s="0" t="n">
         <f aca="false">ROUNDDOWN(N23/E23,0)</f>
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="P23" s="0" t="n">
         <f aca="false">MIN((ROUNDDOWN(N23,0)),ROUNDDOWN(((((M23)/1000)*80)-(60*(D23/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q23" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P23/2,0)</f>
-        <v>67</v>
+        <v>150</v>
       </c>
       <c r="R23" s="11"/>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="6" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E24" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F24" s="8" t="n">
-        <f aca="false">200*(D24/1000)+50*((D24/1000)-0.3)*(E24-1)</f>
-        <v>420</v>
-      </c>
-      <c r="G24" s="5" t="n">
-        <f aca="false">ROUNDDOWN(F24/E24,0)</f>
-        <v>70</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I24" s="0" t="n">
-        <v>850</v>
-      </c>
-      <c r="J24" s="5" t="n">
-        <f aca="false" t="array" ref="J24:J24">_xlfn.IFS(AND($I24&gt;=$M$6,$I24&lt;$M$7),$N$6,AND($I24&gt;=$M$7,$I24&lt;$M$8),$N$7,$I24&gt;=$M$8,$N$8+($I24-$M$8)/5)</f>
-        <v>110</v>
-      </c>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="5"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="M24" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="N24" s="5" t="n">
-        <f aca="false" t="array" ref="N24:N24">_xlfn.IFS(AND($M24&gt;=$M$6,$M24&lt;$M$7),$N$6,AND($M24&gt;=$M$7,$M24&lt;$M$8),$N$7,$M24&gt;=$M$8,$N$8+($M24-$M$8)/5)</f>
-        <v>310</v>
-      </c>
-      <c r="O24" s="0" t="n">
-        <f aca="false">ROUNDDOWN(N24/E24,0)</f>
-        <v>51</v>
-      </c>
-      <c r="P24" s="0" t="n">
-        <f aca="false">MIN((ROUNDDOWN(N24,0)),ROUNDDOWN((((M24/1000)*80)-(60*(D24/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q24" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P24/2,0)</f>
-        <v>67</v>
-      </c>
+      <c r="M24" s="9"/>
+      <c r="N24" s="5"/>
       <c r="R24" s="11"/>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
-        <v>43</v>
-      </c>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="6" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E25" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F25" s="8" t="n">
-        <f aca="false">200*(D25/1000)+50*((D25/1000)-0.3)*(E25-1)</f>
-        <v>420</v>
-      </c>
-      <c r="G25" s="5" t="n">
-        <f aca="false">ROUNDDOWN(F25/E25,0)</f>
-        <v>70</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>38</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
       <c r="I25" s="0" t="n">
-        <v>850</v>
+        <v>1050</v>
       </c>
       <c r="J25" s="5" t="n">
         <f aca="false" t="array" ref="J25:J25">_xlfn.IFS(AND($I25&gt;=$M$6,$I25&lt;$M$7),$N$6,AND($I25&gt;=$M$7,$I25&lt;$M$8),$N$7,$I25&gt;=$M$8,$N$8+($I25-$M$8)/5)</f>
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="K25" s="5"/>
-      <c r="M25" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="N25" s="5" t="n">
-        <f aca="false" t="array" ref="N25:N25">_xlfn.IFS(AND($M25&gt;=$M$6,$M25&lt;$M$7),$N$6,AND($M25&gt;=$M$7,$M25&lt;$M$8),$N$7,$M25&gt;=$M$8,$N$8+($M25-$M$8)/5)</f>
-        <v>310</v>
-      </c>
-      <c r="O25" s="0" t="n">
-        <f aca="false">ROUNDDOWN(N25/E25,0)</f>
-        <v>51</v>
-      </c>
-      <c r="P25" s="0" t="n">
-        <f aca="false">MIN((ROUNDDOWN(N25,0)),ROUNDDOWN((((M25/1000)*80)-(60*(D25/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q25" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P25/2,0)</f>
-        <v>67</v>
-      </c>
+      <c r="M25" s="9"/>
+      <c r="N25" s="5"/>
       <c r="R25" s="11"/>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
-        <v>43</v>
-      </c>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="6" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E26" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F26" s="8" t="n">
-        <f aca="false">200*(D26/1000)+50*((D26/1000)-0.3)*(E26-1)</f>
-        <v>420</v>
-      </c>
-      <c r="G26" s="5" t="n">
-        <f aca="false">ROUNDDOWN(F26/E26,0)</f>
-        <v>70</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>38</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
       <c r="I26" s="0" t="n">
-        <v>850</v>
+        <v>1050</v>
       </c>
       <c r="J26" s="5" t="n">
         <f aca="false" t="array" ref="J26:J26">_xlfn.IFS(AND($I26&gt;=$M$6,$I26&lt;$M$7),$N$6,AND($I26&gt;=$M$7,$I26&lt;$M$8),$N$7,$I26&gt;=$M$8,$N$8+($I26-$M$8)/5)</f>
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="K26" s="5"/>
-      <c r="M26" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="N26" s="5" t="n">
-        <f aca="false" t="array" ref="N26:N26">_xlfn.IFS(AND($M26&gt;=$M$6,$M26&lt;$M$7),$N$6,AND($M26&gt;=$M$7,$M26&lt;$M$8),$N$7,$M26&gt;=$M$8,$N$8+($M26-$M$8)/5)</f>
-        <v>310</v>
-      </c>
-      <c r="O26" s="0" t="n">
-        <f aca="false">ROUNDDOWN(N26/E26,0)</f>
-        <v>51</v>
-      </c>
-      <c r="P26" s="0" t="n">
-        <f aca="false">MIN((ROUNDDOWN(N26,0)),ROUNDDOWN(((((M26)/1000)*80)-(60*(D26/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q26" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P26/2,0)</f>
-        <v>67</v>
-      </c>
+      <c r="M26" s="9"/>
+      <c r="N26" s="5"/>
       <c r="R26" s="11"/>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" s="6" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E27" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F27" s="8" t="n">
-        <f aca="false">200*(D27/1000)+50*((D27/1000)-0.3)*(E27-1)</f>
-        <v>420</v>
-      </c>
-      <c r="G27" s="5" t="n">
-        <f aca="false">ROUNDDOWN(F27/E27,0)</f>
-        <v>70</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I27" s="0" t="n">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="5"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="5"/>
+      <c r="R27" s="11"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="6" t="n">
+        <f aca="false">SUM(G20:G23, J25:J26)-MAX(G20:G23,J25:J26)</f>
+        <v>572</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="6" t="n">
+        <f aca="false">SUM(P20:P23, J25:J26)-MAX(P20:P23,J25:J26)</f>
         <v>850</v>
       </c>
-      <c r="J27" s="5" t="n">
-        <f aca="false" t="array" ref="J27:J27">_xlfn.IFS(AND($I27&gt;=$M$6,$I27&lt;$M$7),$N$6,AND($I27&gt;=$M$7,$I27&lt;$M$8),$N$7,$I27&gt;=$M$8,$N$8+($I27-$M$8)/5)</f>
-        <v>110</v>
-      </c>
-      <c r="K27" s="5"/>
-      <c r="M27" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="N27" s="5" t="n">
-        <f aca="false" t="array" ref="N27:N27">_xlfn.IFS(AND($M27&gt;=$M$6,$M27&lt;$M$7),$N$6,AND($M27&gt;=$M$7,$M27&lt;$M$8),$N$7,$M27&gt;=$M$8,$N$8+($M27-$M$8)/5)</f>
-        <v>310</v>
-      </c>
-      <c r="O27" s="0" t="n">
-        <f aca="false">ROUNDDOWN(N27/E27,0)</f>
-        <v>51</v>
-      </c>
-      <c r="P27" s="0" t="n">
-        <f aca="false">MIN((ROUNDDOWN(N27,0)),ROUNDDOWN(((((M27)/1000)*80)-(60*(D27/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q27" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P27/2,0)</f>
-        <v>67</v>
-      </c>
-      <c r="R27" s="11"/>
-    </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="6" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E28" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F28" s="8" t="n">
-        <f aca="false">200*(D28/1000)+50*((D28/1000)-0.3)*(E28-1)</f>
-        <v>340</v>
-      </c>
-      <c r="G28" s="5" t="n">
-        <f aca="false">ROUNDDOWN(F28/E28,0)</f>
-        <v>85</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I28" s="0" t="n">
-        <v>850</v>
-      </c>
-      <c r="J28" s="5" t="n">
-        <f aca="false" t="array" ref="J28:J28">_xlfn.IFS(AND($I28&gt;=$M$6,$I28&lt;$M$7),$N$6,AND($I28&gt;=$M$7,$I28&lt;$M$8),$N$7,$I28&gt;=$M$8,$N$8+($I28-$M$8)/5)</f>
-        <v>110</v>
-      </c>
-      <c r="K28" s="5"/>
-      <c r="M28" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="N28" s="5" t="n">
-        <f aca="false" t="array" ref="N28:N28">_xlfn.IFS(AND($M28&gt;=$M$6,$M28&lt;$M$7),$N$6,AND($M28&gt;=$M$7,$M28&lt;$M$8),$N$7,$M28&gt;=$M$8,$N$8+($M28-$M$8)/5)</f>
-        <v>310</v>
-      </c>
-      <c r="O28" s="0" t="n">
-        <f aca="false">ROUNDDOWN(N28/E28,0)</f>
-        <v>77</v>
-      </c>
-      <c r="P28" s="0" t="n">
-        <f aca="false">MIN((ROUNDDOWN(N28,0)),ROUNDDOWN((((M28/1000)*80)-(60*(D28/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q28" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P28/2,0)</f>
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="6" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E29" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F29" s="8" t="n">
-        <f aca="false">200*(D29/1000)+50*((D29/1000)-0.3)*(E29-1)</f>
-        <v>340</v>
-      </c>
-      <c r="G29" s="5" t="n">
-        <f aca="false">ROUNDDOWN(F29/E29,0)</f>
-        <v>85</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I29" s="0" t="n">
-        <v>850</v>
-      </c>
-      <c r="J29" s="5" t="n">
-        <f aca="false" t="array" ref="J29:J29">_xlfn.IFS(AND($I29&gt;=$M$6,$I29&lt;$M$7),$N$6,AND($I29&gt;=$M$7,$I29&lt;$M$8),$N$7,$I29&gt;=$M$8,$N$8+($I29-$M$8)/5)</f>
-        <v>110</v>
-      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="M29" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="N29" s="5" t="n">
-        <f aca="false" t="array" ref="N29:N29">_xlfn.IFS(AND($M29&gt;=$M$6,$M29&lt;$M$7),$N$6,AND($M29&gt;=$M$7,$M29&lt;$M$8),$N$7,$M29&gt;=$M$8,$N$8+($M29-$M$8)/5)</f>
-        <v>310</v>
-      </c>
-      <c r="O29" s="0" t="n">
-        <f aca="false">ROUNDDOWN(N29/E29,0)</f>
-        <v>77</v>
-      </c>
-      <c r="P29" s="0" t="n">
-        <f aca="false">MIN((ROUNDDOWN(N29,0)),ROUNDDOWN(((((M29)/1000)*80)-(60*(D29/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q29" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P29/2,0)</f>
-        <v>67</v>
-      </c>
+      <c r="M29" s="9"/>
+      <c r="N29" s="5"/>
       <c r="R29" s="11"/>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="6" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E30" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F30" s="8" t="n">
-        <f aca="false">200*(D30/1000)+50*((D30/1000)-0.3)*(E30-1)</f>
-        <v>340</v>
-      </c>
-      <c r="G30" s="5" t="n">
-        <f aca="false">ROUNDDOWN(F30/E30,0)</f>
-        <v>85</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I30" s="0" t="n">
-        <v>850</v>
-      </c>
-      <c r="J30" s="5" t="n">
-        <f aca="false" t="array" ref="J30:J30">_xlfn.IFS(AND($I30&gt;=$M$6,$I30&lt;$M$7),$N$6,AND($I30&gt;=$M$7,$I30&lt;$M$8),$N$7,$I30&gt;=$M$8,$N$8+($I30-$M$8)/5)</f>
-        <v>110</v>
-      </c>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="J30" s="5"/>
       <c r="K30" s="5"/>
-      <c r="M30" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="N30" s="5" t="n">
-        <f aca="false" t="array" ref="N30:N30">_xlfn.IFS(AND($M30&gt;=$M$6,$M30&lt;$M$7),$N$6,AND($M30&gt;=$M$7,$M30&lt;$M$8),$N$7,$M30&gt;=$M$8,$N$8+($M30-$M$8)/5)</f>
-        <v>310</v>
-      </c>
-      <c r="O30" s="0" t="n">
-        <f aca="false">ROUNDDOWN(N30/E30,0)</f>
-        <v>77</v>
-      </c>
-      <c r="P30" s="0" t="n">
-        <f aca="false">MIN((ROUNDDOWN(N30,0)),ROUNDDOWN(((((M30)/1000)*80)-(60*(D30/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q30" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P30/2,0)</f>
-        <v>67</v>
-      </c>
+      <c r="M30" s="9"/>
+      <c r="N30" s="5"/>
       <c r="R30" s="11"/>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="6" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E31" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F31" s="8" t="n">
-        <f aca="false">200*(D31/1000)+50*((D31/1000)-0.3)*(E31-1)</f>
-        <v>340</v>
-      </c>
-      <c r="G31" s="5" t="n">
-        <f aca="false">ROUNDDOWN(F31/E31,0)</f>
-        <v>85</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I31" s="0" t="n">
-        <v>850</v>
-      </c>
-      <c r="J31" s="5" t="n">
-        <f aca="false" t="array" ref="J31:J31">_xlfn.IFS(AND($I31&gt;=$M$6,$I31&lt;$M$7),$N$6,AND($I31&gt;=$M$7,$I31&lt;$M$8),$N$7,$I31&gt;=$M$8,$N$8+($I31-$M$8)/5)</f>
-        <v>110</v>
-      </c>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="5"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="J31" s="5"/>
       <c r="K31" s="5"/>
-      <c r="M31" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="N31" s="5" t="n">
-        <f aca="false" t="array" ref="N31:N31">_xlfn.IFS(AND($M31&gt;=$M$6,$M31&lt;$M$7),$N$6,AND($M31&gt;=$M$7,$M31&lt;$M$8),$N$7,$M31&gt;=$M$8,$N$8+($M31-$M$8)/5)</f>
-        <v>310</v>
-      </c>
-      <c r="O31" s="0" t="n">
-        <f aca="false">ROUNDDOWN(N31/E31,0)</f>
-        <v>77</v>
-      </c>
-      <c r="P31" s="0" t="n">
-        <f aca="false">MIN((ROUNDDOWN(N31,0)),ROUNDDOWN((((M31/1000)*80)-(60*(D31/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q31" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P31/2,0)</f>
-        <v>67</v>
-      </c>
+      <c r="M31" s="9"/>
+      <c r="N31" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G34" s="1"/>
@@ -3542,15 +3251,15 @@
       </c>
       <c r="C36" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;C$35,$P$20:$P$31)-_xlfn.MAXIFS($P$20:$P$31,$B$20:$B$31,"="&amp;C$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>540</v>
+        <v>630</v>
       </c>
       <c r="D36" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;D$35,$P$20:$P$31)-_xlfn.MAXIFS($P$20:$P$31,$B$20:$B$31,"="&amp;D$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>540</v>
+        <v>0</v>
       </c>
       <c r="E36" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;E$35,$P$20:$P$31)-_xlfn.MAXIFS($P$20:$P$31,$B$20:$B$31,"="&amp;E$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>540</v>
+        <v>0</v>
       </c>
       <c r="F36" s="14"/>
       <c r="H36" s="14" t="s">
@@ -3576,231 +3285,231 @@
       <c r="B37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="16" t="n">
+      <c r="C37" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;C$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;C$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="D37" s="16" t="n">
+        <v>352</v>
+      </c>
+      <c r="D37" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;D$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;D$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="E37" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;E$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;E$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>340</v>
-      </c>
-      <c r="M37" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M37" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="N37" s="18" t="n">
+      <c r="N37" s="17" t="n">
         <v>3300</v>
       </c>
-      <c r="O37" s="18" t="n">
+      <c r="O37" s="17" t="n">
         <f aca="false">N37/6</f>
         <v>550</v>
       </c>
-      <c r="P37" s="18" t="n">
+      <c r="P37" s="17" t="n">
         <f aca="false">N37/10</f>
         <v>330</v>
       </c>
-      <c r="Q37" s="19" t="n">
+      <c r="Q37" s="18" t="n">
         <f aca="false">N37/SUM(C42:E42)</f>
-        <v>5.89285714285714</v>
+        <v>9.375</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="16" t="n">
+      <c r="C38" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;C$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;C$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="D38" s="16" t="n">
+        <v>352</v>
+      </c>
+      <c r="D38" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;D$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;D$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="E38" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;E$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;E$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>340</v>
-      </c>
-      <c r="M38" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M38" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="N38" s="18" t="n">
+      <c r="N38" s="17" t="n">
         <v>4680</v>
       </c>
-      <c r="O38" s="18" t="n">
+      <c r="O38" s="17" t="n">
         <f aca="false">N38/6</f>
         <v>780</v>
       </c>
-      <c r="P38" s="18" t="n">
+      <c r="P38" s="17" t="n">
         <f aca="false">N38/10</f>
         <v>468</v>
       </c>
-      <c r="Q38" s="19" t="n">
+      <c r="Q38" s="18" t="n">
         <f aca="false">N38/SUM(C41:E41)</f>
-        <v>8.35714285714286</v>
+        <v>13.2954545454545</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="16" t="n">
+      <c r="C39" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;C$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;C$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="D39" s="16" t="n">
+        <v>352</v>
+      </c>
+      <c r="D39" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;D$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;D$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="E39" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;E$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;E$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>340</v>
-      </c>
-      <c r="M39" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="N39" s="18" t="n">
+      <c r="N39" s="17" t="n">
         <v>8060</v>
       </c>
-      <c r="O39" s="18" t="n">
+      <c r="O39" s="17" t="n">
         <f aca="false">N39/6</f>
         <v>1343.33333333333</v>
       </c>
-      <c r="P39" s="18" t="n">
+      <c r="P39" s="17" t="n">
         <f aca="false">N39/10</f>
         <v>806</v>
       </c>
-      <c r="Q39" s="19" t="n">
+      <c r="Q39" s="18" t="n">
         <f aca="false">N39/SUM(C40:E40)</f>
-        <v>8.95555555555556</v>
+        <v>22.8977272727273</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="16" t="n">
+      <c r="C40" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;C$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;C$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="D40" s="16" t="n">
+        <v>352</v>
+      </c>
+      <c r="D40" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;D$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;D$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="E40" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;E$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;E$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>340</v>
-      </c>
-      <c r="M40" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="N40" s="18" t="n">
+      <c r="N40" s="17" t="n">
         <v>8060</v>
       </c>
-      <c r="O40" s="18" t="n">
+      <c r="O40" s="17" t="n">
         <f aca="false">N40/6</f>
         <v>1343.33333333333</v>
       </c>
-      <c r="P40" s="18" t="n">
+      <c r="P40" s="17" t="n">
         <f aca="false">N40/10</f>
         <v>806</v>
       </c>
-      <c r="Q40" s="19" t="n">
+      <c r="Q40" s="18" t="n">
         <f aca="false">N40/SUM(C39:E39)</f>
-        <v>8.95555555555556</v>
+        <v>22.8977272727273</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="16" t="n">
+      <c r="C41" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;C$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;C$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="D41" s="16" t="n">
+        <v>352</v>
+      </c>
+      <c r="D41" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;D$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;D$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="E41" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="M41" s="17" t="n">
+      <c r="M41" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="N41" s="18" t="n">
+      <c r="N41" s="17" t="n">
         <v>8060</v>
       </c>
-      <c r="O41" s="18" t="n">
+      <c r="O41" s="17" t="n">
         <f aca="false">N41/6</f>
         <v>1343.33333333333</v>
       </c>
-      <c r="P41" s="18" t="n">
+      <c r="P41" s="17" t="n">
         <f aca="false">N41/10</f>
         <v>806</v>
       </c>
-      <c r="Q41" s="19" t="n">
+      <c r="Q41" s="18" t="n">
         <f aca="false">N41/SUM(C38:E38)</f>
-        <v>8.95555555555556</v>
+        <v>22.8977272727273</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="16" t="n">
+      <c r="C42" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;C$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;C$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="D42" s="16" t="n">
+        <v>352</v>
+      </c>
+      <c r="D42" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;D$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;D$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="E42" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="M42" s="17" t="n">
+      <c r="M42" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="N42" s="18" t="n">
+      <c r="N42" s="17" t="n">
         <v>7960</v>
       </c>
-      <c r="O42" s="18" t="n">
+      <c r="O42" s="17" t="n">
         <f aca="false">N42/6</f>
         <v>1326.66666666667</v>
       </c>
-      <c r="P42" s="18" t="n">
+      <c r="P42" s="17" t="n">
         <f aca="false">N42/10</f>
         <v>796</v>
       </c>
-      <c r="Q42" s="19" t="n">
+      <c r="Q42" s="18" t="n">
         <f aca="false">N42/SUM(C37:E37)</f>
-        <v>8.84444444444445</v>
+        <v>22.6136363636364</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="M43" s="17" t="s">
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="M43" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="N43" s="18" t="n">
+      <c r="N43" s="17" t="n">
         <v>7380</v>
       </c>
-      <c r="O43" s="18" t="n">
+      <c r="O43" s="17" t="n">
         <f aca="false">N43/6</f>
         <v>1230</v>
       </c>
-      <c r="P43" s="18" t="n">
+      <c r="P43" s="17" t="n">
         <f aca="false">N43/10</f>
         <v>738</v>
       </c>
-      <c r="Q43" s="19" t="n">
+      <c r="Q43" s="18" t="n">
         <f aca="false">N43/SUM(C36:E36)</f>
-        <v>4.55555555555556</v>
+        <v>11.7142857142857</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3809,44 +3518,44 @@
       </c>
       <c r="C44" s="12" t="n">
         <f aca="false">SUM(C36:C42)</f>
-        <v>2220</v>
+        <v>2742</v>
       </c>
       <c r="D44" s="12" t="n">
         <f aca="false">SUM(D36:D42)</f>
-        <v>2220</v>
+        <v>0</v>
       </c>
       <c r="E44" s="12" t="n">
         <f aca="false">SUM(E36:E42)</f>
-        <v>1900</v>
+        <v>0</v>
       </c>
       <c r="G44" s="1"/>
-      <c r="M44" s="17" t="s">
+      <c r="M44" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="N44" s="18" t="n">
+      <c r="N44" s="17" t="n">
         <f aca="false">SUM(N37:N43)</f>
         <v>47500</v>
       </c>
-      <c r="O44" s="18" t="n">
+      <c r="O44" s="17" t="n">
         <f aca="false">SUM(O37:O43)</f>
         <v>7916.66666666667</v>
       </c>
-      <c r="P44" s="18" t="n">
+      <c r="P44" s="17" t="n">
         <f aca="false">SUM(P37:P43)</f>
         <v>4750</v>
       </c>
-      <c r="Q44" s="19" t="e">
+      <c r="Q44" s="18" t="e">
         <f aca="false">N44/SUM(C49:E49)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="20" t="n">
+      <c r="C45" s="19" t="n">
         <f aca="false">SUM(C44:E44)</f>
-        <v>6340</v>
-      </c>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
+        <v>2742</v>
+      </c>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Merged PR 8: MoECapacityCalcService implemented
</commit_message>
<xml_diff>
--- a/ExcelTestData/AreaHMoECapacityTest2.xlsx
+++ b/ExcelTestData/AreaHMoECapacityTest2.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="91">
   <si>
     <t xml:space="preserve">Stair capacity factors</t>
   </si>
@@ -377,6 +377,21 @@
   </si>
   <si>
     <t xml:space="preserve">Merging flow capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StoreyExit 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FinalExit 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If Area is on upper floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacity = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If Area is on final exit level of all stairs</t>
   </si>
 </sst>
 </file>
@@ -506,7 +521,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -569,10 +584,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -702,9 +713,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>64440</xdr:colOff>
+      <xdr:colOff>64080</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>14400</xdr:rowOff>
+      <xdr:rowOff>14040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -717,8 +728,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15707880" y="2081520"/>
-          <a:ext cx="3156480" cy="1009440"/>
+          <a:off x="16114680" y="2081520"/>
+          <a:ext cx="3157560" cy="1009080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -744,7 +755,7 @@
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.17"/>
@@ -757,7 +768,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="31.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="27.46"/>
@@ -2057,33 +2068,33 @@
       <c r="B40" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="16" t="n">
+      <c r="C40" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;C$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;C$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="D40" s="16" t="n">
+      <c r="D40" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;D$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;D$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="E40" s="16" t="n">
+      <c r="E40" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;E$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;E$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>528</v>
       </c>
-      <c r="M40" s="17" t="s">
+      <c r="M40" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="N40" s="18" t="n">
+      <c r="N40" s="17" t="n">
         <v>3300</v>
       </c>
-      <c r="O40" s="18" t="n">
+      <c r="O40" s="17" t="n">
         <f aca="false">N40/6</f>
         <v>550</v>
       </c>
-      <c r="P40" s="18" t="n">
+      <c r="P40" s="17" t="n">
         <f aca="false">N40/10</f>
         <v>330</v>
       </c>
-      <c r="Q40" s="19" t="n">
+      <c r="Q40" s="18" t="n">
         <f aca="false">N40/SUM(C45:E45)</f>
         <v>3.85514018691589</v>
       </c>
@@ -2092,33 +2103,33 @@
       <c r="B41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="16" t="n">
+      <c r="C41" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;C$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;C$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="D41" s="16" t="n">
+      <c r="D41" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;D$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;D$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="E41" s="16" t="n">
+      <c r="E41" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;E$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;E$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>528</v>
       </c>
-      <c r="M41" s="17" t="s">
+      <c r="M41" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="N41" s="18" t="n">
+      <c r="N41" s="17" t="n">
         <v>4680</v>
       </c>
-      <c r="O41" s="18" t="n">
+      <c r="O41" s="17" t="n">
         <f aca="false">N41/6</f>
         <v>780</v>
       </c>
-      <c r="P41" s="18" t="n">
+      <c r="P41" s="17" t="n">
         <f aca="false">N41/10</f>
         <v>468</v>
       </c>
-      <c r="Q41" s="19" t="n">
+      <c r="Q41" s="18" t="n">
         <f aca="false">N41/SUM(C44:E44)</f>
         <v>5.46728971962617</v>
       </c>
@@ -2127,33 +2138,33 @@
       <c r="B42" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C42" s="16" t="n">
+      <c r="C42" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;C$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;C$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="D42" s="16" t="n">
+      <c r="D42" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;D$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;D$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="E42" s="16" t="n">
+      <c r="E42" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;E$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;E$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>528</v>
       </c>
-      <c r="M42" s="17" t="n">
+      <c r="M42" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="N42" s="18" t="n">
+      <c r="N42" s="17" t="n">
         <v>8060</v>
       </c>
-      <c r="O42" s="18" t="n">
+      <c r="O42" s="17" t="n">
         <f aca="false">N42/6</f>
         <v>1343.33333333333</v>
       </c>
-      <c r="P42" s="18" t="n">
+      <c r="P42" s="17" t="n">
         <f aca="false">N42/10</f>
         <v>806</v>
       </c>
-      <c r="Q42" s="19" t="n">
+      <c r="Q42" s="18" t="n">
         <f aca="false">N42/SUM(C43:E43)</f>
         <v>5.82369942196532</v>
       </c>
@@ -2162,33 +2173,33 @@
       <c r="B43" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="16" t="n">
+      <c r="C43" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;C$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;C$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="D43" s="16" t="n">
+      <c r="D43" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;D$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;D$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="E43" s="16" t="n">
+      <c r="E43" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;E$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;E$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>528</v>
       </c>
-      <c r="M43" s="17" t="n">
+      <c r="M43" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="N43" s="18" t="n">
+      <c r="N43" s="17" t="n">
         <v>8060</v>
       </c>
-      <c r="O43" s="18" t="n">
+      <c r="O43" s="17" t="n">
         <f aca="false">N43/6</f>
         <v>1343.33333333333</v>
       </c>
-      <c r="P43" s="18" t="n">
+      <c r="P43" s="17" t="n">
         <f aca="false">N43/10</f>
         <v>806</v>
       </c>
-      <c r="Q43" s="19" t="n">
+      <c r="Q43" s="18" t="n">
         <f aca="false">N43/SUM(C42:E42)</f>
         <v>5.82369942196532</v>
       </c>
@@ -2197,32 +2208,32 @@
       <c r="B44" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C44" s="16" t="n">
+      <c r="C44" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;C$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;C$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="D44" s="16" t="n">
+      <c r="D44" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;D$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;D$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="M44" s="17" t="n">
+      <c r="M44" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="N44" s="18" t="n">
+      <c r="N44" s="17" t="n">
         <v>8060</v>
       </c>
-      <c r="O44" s="18" t="n">
+      <c r="O44" s="17" t="n">
         <f aca="false">N44/6</f>
         <v>1343.33333333333</v>
       </c>
-      <c r="P44" s="18" t="n">
+      <c r="P44" s="17" t="n">
         <f aca="false">N44/10</f>
         <v>806</v>
       </c>
-      <c r="Q44" s="19" t="n">
+      <c r="Q44" s="18" t="n">
         <f aca="false">N44/SUM(C41:E41)</f>
         <v>5.82369942196532</v>
       </c>
@@ -2231,55 +2242,55 @@
       <c r="B45" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C45" s="16" t="n">
+      <c r="C45" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;C$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;C$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="D45" s="16" t="n">
+      <c r="D45" s="13" t="n">
         <f aca="false">SUMIF($B$23:$B$34,"="&amp;D$38,$H$23:$H$34)-_xlfn.MAXIFS($H$23:$H$34,$B$23:$B$34,"="&amp;D$38,$I$23:$I$34,"="&amp;"No")</f>
         <v>428</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="E45" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="M45" s="17" t="n">
+      <c r="M45" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="N45" s="18" t="n">
+      <c r="N45" s="17" t="n">
         <v>7960</v>
       </c>
-      <c r="O45" s="18" t="n">
+      <c r="O45" s="17" t="n">
         <f aca="false">N45/6</f>
         <v>1326.66666666667</v>
       </c>
-      <c r="P45" s="18" t="n">
+      <c r="P45" s="17" t="n">
         <f aca="false">N45/10</f>
         <v>796</v>
       </c>
-      <c r="Q45" s="19" t="n">
+      <c r="Q45" s="18" t="n">
         <f aca="false">N45/SUM(C40:E40)</f>
         <v>5.7514450867052</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="M46" s="17" t="s">
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="M46" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="N46" s="18" t="n">
+      <c r="N46" s="17" t="n">
         <v>7380</v>
       </c>
-      <c r="O46" s="18" t="n">
+      <c r="O46" s="17" t="n">
         <f aca="false">N46/6</f>
         <v>1230</v>
       </c>
-      <c r="P46" s="18" t="n">
+      <c r="P46" s="17" t="n">
         <f aca="false">N46/10</f>
         <v>738</v>
       </c>
-      <c r="Q46" s="19" t="n">
+      <c r="Q46" s="18" t="n">
         <f aca="false">N46/SUM(C39:E39)</f>
         <v>4.07284768211921</v>
       </c>
@@ -2301,33 +2312,33 @@
         <v>2716</v>
       </c>
       <c r="G47" s="1"/>
-      <c r="M47" s="17" t="s">
+      <c r="M47" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="N47" s="18" t="n">
+      <c r="N47" s="17" t="n">
         <f aca="false">SUM(N40:N46)</f>
         <v>47500</v>
       </c>
-      <c r="O47" s="18" t="n">
+      <c r="O47" s="17" t="n">
         <f aca="false">SUM(O40:O46)</f>
         <v>7916.66666666667</v>
       </c>
-      <c r="P47" s="18" t="n">
+      <c r="P47" s="17" t="n">
         <f aca="false">SUM(P40:P46)</f>
         <v>4750</v>
       </c>
-      <c r="Q47" s="19" t="e">
+      <c r="Q47" s="18" t="e">
         <f aca="false">N47/SUM(C52:E52)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="20" t="n">
+      <c r="C48" s="19" t="n">
         <f aca="false">SUM(C47:E47)</f>
         <v>9060</v>
       </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2351,12 +2362,12 @@
   <dimension ref="B1:R45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.82"/>
@@ -2369,7 +2380,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.91"/>
   </cols>
   <sheetData>
@@ -2393,14 +2404,14 @@
         <v>75</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="H2" s="0" t="n">
         <f aca="false">200*(G2/1000)+50*((G2/1000)-0.3)*(F2-1)</f>
-        <v>645</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2413,18 +2424,18 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="19"/>
-      <c r="C5" s="21" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
       <c r="M5" s="1" t="s">
         <v>78</v>
       </c>
@@ -2436,41 +2447,41 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="23" t="n">
+      <c r="C6" s="22" t="n">
         <v>1000</v>
       </c>
-      <c r="D6" s="23" t="n">
+      <c r="D6" s="22" t="n">
         <f aca="false">C6+100</f>
         <v>1100</v>
       </c>
-      <c r="E6" s="23" t="n">
+      <c r="E6" s="22" t="n">
         <f aca="false">D6+100</f>
         <v>1200</v>
       </c>
-      <c r="F6" s="23" t="n">
+      <c r="F6" s="22" t="n">
         <f aca="false">E6+100</f>
         <v>1300</v>
       </c>
-      <c r="G6" s="23" t="n">
+      <c r="G6" s="22" t="n">
         <f aca="false">F6+100</f>
         <v>1400</v>
       </c>
-      <c r="H6" s="23" t="n">
+      <c r="H6" s="22" t="n">
         <f aca="false">G6+100</f>
         <v>1500</v>
       </c>
-      <c r="I6" s="23" t="n">
+      <c r="I6" s="22" t="n">
         <f aca="false">H6+100</f>
         <v>1600</v>
       </c>
-      <c r="J6" s="23" t="n">
+      <c r="J6" s="22" t="n">
         <f aca="false">I6+100</f>
         <v>1700</v>
       </c>
-      <c r="K6" s="23" t="n">
+      <c r="K6" s="22" t="n">
         <f aca="false">J6+100</f>
         <v>1800</v>
       </c>
@@ -2485,34 +2496,34 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="22" t="n">
+      <c r="B7" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="24" t="n">
+      <c r="C7" s="23" t="n">
         <v>150</v>
       </c>
-      <c r="D7" s="24" t="n">
+      <c r="D7" s="23" t="n">
         <v>220</v>
       </c>
-      <c r="E7" s="24" t="n">
+      <c r="E7" s="23" t="n">
         <v>240</v>
       </c>
-      <c r="F7" s="24" t="n">
+      <c r="F7" s="23" t="n">
         <v>260</v>
       </c>
-      <c r="G7" s="24" t="n">
+      <c r="G7" s="23" t="n">
         <v>280</v>
       </c>
-      <c r="H7" s="24" t="n">
+      <c r="H7" s="23" t="n">
         <v>300</v>
       </c>
-      <c r="I7" s="24" t="n">
+      <c r="I7" s="23" t="n">
         <v>320</v>
       </c>
-      <c r="J7" s="24" t="n">
+      <c r="J7" s="23" t="n">
         <v>340</v>
       </c>
-      <c r="K7" s="24" t="n">
+      <c r="K7" s="23" t="n">
         <v>360</v>
       </c>
       <c r="M7" s="1" t="n">
@@ -2526,34 +2537,34 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="22" t="n">
+      <c r="B8" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="24" t="n">
+      <c r="C8" s="23" t="n">
         <v>190</v>
       </c>
-      <c r="D8" s="24" t="n">
+      <c r="D8" s="23" t="n">
         <v>260</v>
       </c>
-      <c r="E8" s="24" t="n">
+      <c r="E8" s="23" t="n">
         <v>285</v>
       </c>
-      <c r="F8" s="24" t="n">
+      <c r="F8" s="23" t="n">
         <v>310</v>
       </c>
-      <c r="G8" s="24" t="n">
+      <c r="G8" s="23" t="n">
         <v>335</v>
       </c>
-      <c r="H8" s="24" t="n">
+      <c r="H8" s="23" t="n">
         <v>360</v>
       </c>
-      <c r="I8" s="24" t="n">
+      <c r="I8" s="23" t="n">
         <v>385</v>
       </c>
-      <c r="J8" s="24" t="n">
+      <c r="J8" s="23" t="n">
         <v>410</v>
       </c>
-      <c r="K8" s="24" t="n">
+      <c r="K8" s="23" t="n">
         <v>435</v>
       </c>
       <c r="M8" s="1" t="n">
@@ -2567,37 +2578,37 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="22" t="n">
+      <c r="B9" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="24" t="n">
+      <c r="C9" s="23" t="n">
         <v>230</v>
       </c>
-      <c r="D9" s="24" t="n">
+      <c r="D9" s="23" t="n">
         <v>300</v>
       </c>
-      <c r="E9" s="24" t="n">
+      <c r="E9" s="23" t="n">
         <v>330</v>
       </c>
-      <c r="F9" s="24" t="n">
+      <c r="F9" s="23" t="n">
         <v>360</v>
       </c>
-      <c r="G9" s="24" t="n">
+      <c r="G9" s="23" t="n">
         <v>390</v>
       </c>
-      <c r="H9" s="24" t="n">
+      <c r="H9" s="23" t="n">
         <v>420</v>
       </c>
-      <c r="I9" s="24" t="n">
+      <c r="I9" s="23" t="n">
         <v>450</v>
       </c>
-      <c r="J9" s="24" t="n">
+      <c r="J9" s="23" t="n">
         <v>480</v>
       </c>
-      <c r="K9" s="24" t="n">
+      <c r="K9" s="23" t="n">
         <v>510</v>
       </c>
-      <c r="M9" s="25" t="s">
+      <c r="M9" s="24" t="s">
         <v>81</v>
       </c>
       <c r="N9" s="3" t="s">
@@ -2608,228 +2619,228 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="22" t="n">
+      <c r="B10" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="24" t="n">
+      <c r="C10" s="23" t="n">
         <v>270</v>
       </c>
-      <c r="D10" s="24" t="n">
+      <c r="D10" s="23" t="n">
         <v>340</v>
       </c>
-      <c r="E10" s="24" t="n">
+      <c r="E10" s="23" t="n">
         <v>375</v>
       </c>
-      <c r="F10" s="24" t="n">
+      <c r="F10" s="23" t="n">
         <v>410</v>
       </c>
-      <c r="G10" s="24" t="n">
+      <c r="G10" s="23" t="n">
         <v>445</v>
       </c>
-      <c r="H10" s="24" t="n">
+      <c r="H10" s="23" t="n">
         <v>480</v>
       </c>
-      <c r="I10" s="24" t="n">
+      <c r="I10" s="23" t="n">
         <v>515</v>
       </c>
-      <c r="J10" s="24" t="n">
+      <c r="J10" s="23" t="n">
         <v>550</v>
       </c>
-      <c r="K10" s="24" t="n">
+      <c r="K10" s="23" t="n">
         <v>585</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="22" t="n">
+      <c r="B11" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="24" t="n">
+      <c r="C11" s="23" t="n">
         <v>310</v>
       </c>
-      <c r="D11" s="24" t="n">
+      <c r="D11" s="23" t="n">
         <v>380</v>
       </c>
-      <c r="E11" s="24" t="n">
+      <c r="E11" s="23" t="n">
         <v>420</v>
       </c>
-      <c r="F11" s="24" t="n">
+      <c r="F11" s="23" t="n">
         <v>460</v>
       </c>
-      <c r="G11" s="24" t="n">
+      <c r="G11" s="23" t="n">
         <v>500</v>
       </c>
-      <c r="H11" s="24" t="n">
+      <c r="H11" s="23" t="n">
         <v>540</v>
       </c>
-      <c r="I11" s="24" t="n">
+      <c r="I11" s="23" t="n">
         <v>580</v>
       </c>
-      <c r="J11" s="24" t="n">
+      <c r="J11" s="23" t="n">
         <v>620</v>
       </c>
-      <c r="K11" s="24" t="n">
+      <c r="K11" s="23" t="n">
         <v>660</v>
       </c>
       <c r="L11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="22" t="n">
+      <c r="B12" s="21" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="24" t="n">
+      <c r="C12" s="23" t="n">
         <v>350</v>
       </c>
-      <c r="D12" s="24" t="n">
+      <c r="D12" s="23" t="n">
         <v>420</v>
       </c>
-      <c r="E12" s="24" t="n">
+      <c r="E12" s="23" t="n">
         <v>465</v>
       </c>
-      <c r="F12" s="24" t="n">
+      <c r="F12" s="23" t="n">
         <v>510</v>
       </c>
-      <c r="G12" s="24" t="n">
+      <c r="G12" s="23" t="n">
         <v>555</v>
       </c>
-      <c r="H12" s="24" t="n">
+      <c r="H12" s="23" t="n">
         <v>600</v>
       </c>
-      <c r="I12" s="24" t="n">
+      <c r="I12" s="23" t="n">
         <v>645</v>
       </c>
-      <c r="J12" s="24" t="n">
+      <c r="J12" s="23" t="n">
         <v>690</v>
       </c>
-      <c r="K12" s="24" t="n">
+      <c r="K12" s="23" t="n">
         <v>735</v>
       </c>
       <c r="L12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="22" t="n">
+      <c r="B13" s="21" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="24" t="n">
+      <c r="C13" s="23" t="n">
         <v>390</v>
       </c>
-      <c r="D13" s="24" t="n">
+      <c r="D13" s="23" t="n">
         <v>460</v>
       </c>
-      <c r="E13" s="24" t="n">
+      <c r="E13" s="23" t="n">
         <v>510</v>
       </c>
-      <c r="F13" s="24" t="n">
+      <c r="F13" s="23" t="n">
         <v>560</v>
       </c>
-      <c r="G13" s="24" t="n">
+      <c r="G13" s="23" t="n">
         <v>610</v>
       </c>
-      <c r="H13" s="24" t="n">
+      <c r="H13" s="23" t="n">
         <v>660</v>
       </c>
-      <c r="I13" s="24" t="n">
+      <c r="I13" s="23" t="n">
         <v>710</v>
       </c>
-      <c r="J13" s="24" t="n">
+      <c r="J13" s="23" t="n">
         <v>760</v>
       </c>
-      <c r="K13" s="24" t="n">
+      <c r="K13" s="23" t="n">
         <v>810</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="22" t="n">
+      <c r="B14" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="24" t="n">
+      <c r="C14" s="23" t="n">
         <v>430</v>
       </c>
-      <c r="D14" s="24" t="n">
+      <c r="D14" s="23" t="n">
         <v>500</v>
       </c>
-      <c r="E14" s="24" t="n">
+      <c r="E14" s="23" t="n">
         <v>555</v>
       </c>
-      <c r="F14" s="24" t="n">
+      <c r="F14" s="23" t="n">
         <v>610</v>
       </c>
-      <c r="G14" s="24" t="n">
+      <c r="G14" s="23" t="n">
         <v>665</v>
       </c>
-      <c r="H14" s="24" t="n">
+      <c r="H14" s="23" t="n">
         <v>720</v>
       </c>
-      <c r="I14" s="24" t="n">
+      <c r="I14" s="23" t="n">
         <v>775</v>
       </c>
-      <c r="J14" s="24" t="n">
+      <c r="J14" s="23" t="n">
         <v>830</v>
       </c>
-      <c r="K14" s="24" t="n">
+      <c r="K14" s="23" t="n">
         <v>885</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="22" t="n">
+      <c r="B15" s="21" t="n">
         <v>9</v>
       </c>
-      <c r="C15" s="24" t="n">
+      <c r="C15" s="23" t="n">
         <v>470</v>
       </c>
-      <c r="D15" s="24" t="n">
+      <c r="D15" s="23" t="n">
         <v>540</v>
       </c>
-      <c r="E15" s="24" t="n">
+      <c r="E15" s="23" t="n">
         <v>600</v>
       </c>
-      <c r="F15" s="24" t="n">
+      <c r="F15" s="23" t="n">
         <v>660</v>
       </c>
-      <c r="G15" s="24" t="n">
+      <c r="G15" s="23" t="n">
         <v>720</v>
       </c>
-      <c r="H15" s="24" t="n">
+      <c r="H15" s="23" t="n">
         <v>780</v>
       </c>
-      <c r="I15" s="24" t="n">
+      <c r="I15" s="23" t="n">
         <v>840</v>
       </c>
-      <c r="J15" s="24" t="n">
+      <c r="J15" s="23" t="n">
         <v>900</v>
       </c>
-      <c r="K15" s="24" t="n">
+      <c r="K15" s="23" t="n">
         <v>960</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="22" t="n">
+      <c r="B16" s="21" t="n">
         <v>10</v>
       </c>
-      <c r="C16" s="24" t="n">
+      <c r="C16" s="23" t="n">
         <v>510</v>
       </c>
-      <c r="D16" s="24" t="n">
+      <c r="D16" s="23" t="n">
         <v>580</v>
       </c>
-      <c r="E16" s="24" t="n">
+      <c r="E16" s="23" t="n">
         <v>645</v>
       </c>
-      <c r="F16" s="24" t="n">
+      <c r="F16" s="23" t="n">
         <v>710</v>
       </c>
-      <c r="G16" s="24" t="n">
+      <c r="G16" s="23" t="n">
         <v>775</v>
       </c>
-      <c r="H16" s="24" t="n">
+      <c r="H16" s="23" t="n">
         <v>840</v>
       </c>
-      <c r="I16" s="24" t="n">
+      <c r="I16" s="23" t="n">
         <v>905</v>
       </c>
-      <c r="J16" s="24" t="n">
+      <c r="J16" s="23" t="n">
         <v>970</v>
       </c>
-      <c r="K16" s="24" t="n">
+      <c r="K16" s="23" t="n">
         <v>1035</v>
       </c>
     </row>
@@ -2837,42 +2848,42 @@
       <c r="B17" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="26" t="s">
+      <c r="H19" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="I19" s="26" t="s">
+      <c r="I19" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="J19" s="26" t="s">
+      <c r="J19" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="K19" s="26"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="26" t="s">
+      <c r="K19" s="25"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="N19" s="26" t="s">
+      <c r="N19" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="O19" s="26" t="s">
+      <c r="O19" s="25" t="s">
         <v>32</v>
       </c>
       <c r="P19" s="1" t="s">
@@ -2885,7 +2896,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>36</v>
       </c>
@@ -2893,52 +2904,48 @@
         <v>37</v>
       </c>
       <c r="D20" s="6" t="n">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F20" s="8" t="n">
-        <f aca="false">200*(D20/1000)+50*((D20/1000)-0.3)*(E20-1)</f>
-        <v>420</v>
+        <v>230</v>
       </c>
       <c r="G20" s="5" t="n">
         <f aca="false">ROUNDDOWN(F20/E20,0)</f>
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>38</v>
       </c>
       <c r="I20" s="0" t="n">
-        <v>850</v>
+        <v>1050</v>
       </c>
       <c r="J20" s="5" t="n">
         <f aca="false" t="array" ref="J20:J20">_xlfn.IFS(AND($I20&gt;=$M$6,$I20&lt;$M$7),$N$6,AND($I20&gt;=$M$7,$I20&lt;$M$8),$N$7,$I20&gt;=$M$8,$N$8+($I20-$M$8)/5)</f>
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="K20" s="5"/>
       <c r="M20" s="9" t="n">
-        <v>1500</v>
+        <f aca="false">1050+0.5*1050</f>
+        <v>1575</v>
       </c>
       <c r="N20" s="5" t="n">
         <f aca="false" t="array" ref="N20:N20">_xlfn.IFS(AND($M20&gt;=$M$6,$M20&lt;$M$7),$N$6,AND($M20&gt;=$M$7,$M20&lt;$M$8),$N$7,$M20&gt;=$M$8,$N$8+($M20-$M$8)/5)</f>
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="O20" s="0" t="n">
         <f aca="false">ROUNDDOWN(N20/E20,0)</f>
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="P20" s="0" t="n">
         <f aca="false">MIN((ROUNDDOWN(N20,0)),ROUNDDOWN(((((M20)/1000)*80)-(60*(D20/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q20" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P20/2,0)</f>
-        <v>67</v>
+        <v>165</v>
       </c>
       <c r="R20" s="11"/>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
         <v>36</v>
       </c>
@@ -2949,48 +2956,45 @@
         <v>1100</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F21" s="8" t="n">
         <f aca="false">200*(D21/1000)+50*((D21/1000)-0.3)*(E21-1)</f>
-        <v>420</v>
+        <v>300</v>
       </c>
       <c r="G21" s="5" t="n">
         <f aca="false">ROUNDDOWN(F21/E21,0)</f>
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>38</v>
       </c>
       <c r="I21" s="0" t="n">
-        <v>850</v>
+        <v>1050</v>
       </c>
       <c r="J21" s="5" t="n">
         <f aca="false" t="array" ref="J21:J21">_xlfn.IFS(AND($I21&gt;=$M$6,$I21&lt;$M$7),$N$6,AND($I21&gt;=$M$7,$I21&lt;$M$8),$N$7,$I21&gt;=$M$8,$N$8+($I21-$M$8)/5)</f>
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="K21" s="5"/>
       <c r="M21" s="9" t="n">
-        <v>1500</v>
+        <f aca="false">1050+0.5*1050</f>
+        <v>1575</v>
       </c>
       <c r="N21" s="5" t="n">
         <f aca="false" t="array" ref="N21:N21">_xlfn.IFS(AND($M21&gt;=$M$6,$M21&lt;$M$7),$N$6,AND($M21&gt;=$M$7,$M21&lt;$M$8),$N$7,$M21&gt;=$M$8,$N$8+($M21-$M$8)/5)</f>
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="O21" s="0" t="n">
         <f aca="false">ROUNDDOWN(N21/E21,0)</f>
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="P21" s="0" t="n">
         <f aca="false">MIN((ROUNDDOWN(N21,0)),ROUNDDOWN((((M21/1000)*80)-(60*(D21/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q21" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P21/2,0)</f>
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>36</v>
       </c>
@@ -2998,52 +3002,48 @@
         <v>41</v>
       </c>
       <c r="D22" s="6" t="n">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F22" s="8" t="n">
-        <f aca="false">200*(D22/1000)+50*((D22/1000)-0.3)*(E22-1)</f>
-        <v>420</v>
+        <v>230</v>
       </c>
       <c r="G22" s="5" t="n">
         <f aca="false">ROUNDDOWN(F22/E22,0)</f>
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>38</v>
       </c>
       <c r="I22" s="0" t="n">
-        <v>850</v>
+        <v>1050</v>
       </c>
       <c r="J22" s="5" t="n">
         <f aca="false" t="array" ref="J22:J22">_xlfn.IFS(AND($I22&gt;=$M$6,$I22&lt;$M$7),$N$6,AND($I22&gt;=$M$7,$I22&lt;$M$8),$N$7,$I22&gt;=$M$8,$N$8+($I22-$M$8)/5)</f>
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="K22" s="5"/>
       <c r="M22" s="9" t="n">
-        <v>1500</v>
+        <f aca="false">1050+0.5*1050</f>
+        <v>1575</v>
       </c>
       <c r="N22" s="5" t="n">
         <f aca="false" t="array" ref="N22:N22">_xlfn.IFS(AND($M22&gt;=$M$6,$M22&lt;$M$7),$N$6,AND($M22&gt;=$M$7,$M22&lt;$M$8),$N$7,$M22&gt;=$M$8,$N$8+($M22-$M$8)/5)</f>
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="O22" s="0" t="n">
         <f aca="false">ROUNDDOWN(N22/E22,0)</f>
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="P22" s="0" t="n">
         <f aca="false">MIN((ROUNDDOWN(N22,0)),ROUNDDOWN((((M22/1000)*80)-(60*(D22/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q22" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P22/2,0)</f>
-        <v>67</v>
+        <v>165</v>
       </c>
       <c r="R22" s="11"/>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
         <v>36</v>
       </c>
@@ -3054,469 +3054,178 @@
         <v>1100</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F23" s="8" t="n">
         <f aca="false">200*(D23/1000)+50*((D23/1000)-0.3)*(E23-1)</f>
-        <v>420</v>
+        <v>300</v>
       </c>
       <c r="G23" s="5" t="n">
         <f aca="false">ROUNDDOWN(F23/E23,0)</f>
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>38</v>
       </c>
       <c r="I23" s="0" t="n">
-        <v>850</v>
+        <v>1050</v>
       </c>
       <c r="J23" s="5" t="n">
         <f aca="false" t="array" ref="J23:J23">_xlfn.IFS(AND($I23&gt;=$M$6,$I23&lt;$M$7),$N$6,AND($I23&gt;=$M$7,$I23&lt;$M$8),$N$7,$I23&gt;=$M$8,$N$8+($I23-$M$8)/5)</f>
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="K23" s="5"/>
       <c r="M23" s="9" t="n">
-        <v>1500</v>
+        <f aca="false">1050+0.5*1050</f>
+        <v>1575</v>
       </c>
       <c r="N23" s="5" t="n">
         <f aca="false" t="array" ref="N23:N23">_xlfn.IFS(AND($M23&gt;=$M$6,$M23&lt;$M$7),$N$6,AND($M23&gt;=$M$7,$M23&lt;$M$8),$N$7,$M23&gt;=$M$8,$N$8+($M23-$M$8)/5)</f>
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="O23" s="0" t="n">
         <f aca="false">ROUNDDOWN(N23/E23,0)</f>
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="P23" s="0" t="n">
         <f aca="false">MIN((ROUNDDOWN(N23,0)),ROUNDDOWN(((((M23)/1000)*80)-(60*(D23/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q23" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P23/2,0)</f>
-        <v>67</v>
+        <v>150</v>
       </c>
       <c r="R23" s="11"/>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="6" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E24" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F24" s="8" t="n">
-        <f aca="false">200*(D24/1000)+50*((D24/1000)-0.3)*(E24-1)</f>
-        <v>420</v>
-      </c>
-      <c r="G24" s="5" t="n">
-        <f aca="false">ROUNDDOWN(F24/E24,0)</f>
-        <v>70</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I24" s="0" t="n">
-        <v>850</v>
-      </c>
-      <c r="J24" s="5" t="n">
-        <f aca="false" t="array" ref="J24:J24">_xlfn.IFS(AND($I24&gt;=$M$6,$I24&lt;$M$7),$N$6,AND($I24&gt;=$M$7,$I24&lt;$M$8),$N$7,$I24&gt;=$M$8,$N$8+($I24-$M$8)/5)</f>
-        <v>110</v>
-      </c>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="5"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="M24" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="N24" s="5" t="n">
-        <f aca="false" t="array" ref="N24:N24">_xlfn.IFS(AND($M24&gt;=$M$6,$M24&lt;$M$7),$N$6,AND($M24&gt;=$M$7,$M24&lt;$M$8),$N$7,$M24&gt;=$M$8,$N$8+($M24-$M$8)/5)</f>
-        <v>310</v>
-      </c>
-      <c r="O24" s="0" t="n">
-        <f aca="false">ROUNDDOWN(N24/E24,0)</f>
-        <v>51</v>
-      </c>
-      <c r="P24" s="0" t="n">
-        <f aca="false">MIN((ROUNDDOWN(N24,0)),ROUNDDOWN((((M24/1000)*80)-(60*(D24/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q24" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P24/2,0)</f>
-        <v>67</v>
-      </c>
+      <c r="M24" s="9"/>
+      <c r="N24" s="5"/>
       <c r="R24" s="11"/>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
-        <v>43</v>
-      </c>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="6" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E25" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F25" s="8" t="n">
-        <f aca="false">200*(D25/1000)+50*((D25/1000)-0.3)*(E25-1)</f>
-        <v>420</v>
-      </c>
-      <c r="G25" s="5" t="n">
-        <f aca="false">ROUNDDOWN(F25/E25,0)</f>
-        <v>70</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>38</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
       <c r="I25" s="0" t="n">
-        <v>850</v>
+        <v>1050</v>
       </c>
       <c r="J25" s="5" t="n">
         <f aca="false" t="array" ref="J25:J25">_xlfn.IFS(AND($I25&gt;=$M$6,$I25&lt;$M$7),$N$6,AND($I25&gt;=$M$7,$I25&lt;$M$8),$N$7,$I25&gt;=$M$8,$N$8+($I25-$M$8)/5)</f>
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="K25" s="5"/>
-      <c r="M25" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="N25" s="5" t="n">
-        <f aca="false" t="array" ref="N25:N25">_xlfn.IFS(AND($M25&gt;=$M$6,$M25&lt;$M$7),$N$6,AND($M25&gt;=$M$7,$M25&lt;$M$8),$N$7,$M25&gt;=$M$8,$N$8+($M25-$M$8)/5)</f>
-        <v>310</v>
-      </c>
-      <c r="O25" s="0" t="n">
-        <f aca="false">ROUNDDOWN(N25/E25,0)</f>
-        <v>51</v>
-      </c>
-      <c r="P25" s="0" t="n">
-        <f aca="false">MIN((ROUNDDOWN(N25,0)),ROUNDDOWN((((M25/1000)*80)-(60*(D25/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q25" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P25/2,0)</f>
-        <v>67</v>
-      </c>
+      <c r="M25" s="9"/>
+      <c r="N25" s="5"/>
       <c r="R25" s="11"/>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
-        <v>43</v>
-      </c>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="6" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E26" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F26" s="8" t="n">
-        <f aca="false">200*(D26/1000)+50*((D26/1000)-0.3)*(E26-1)</f>
-        <v>420</v>
-      </c>
-      <c r="G26" s="5" t="n">
-        <f aca="false">ROUNDDOWN(F26/E26,0)</f>
-        <v>70</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>38</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
       <c r="I26" s="0" t="n">
-        <v>850</v>
+        <v>1050</v>
       </c>
       <c r="J26" s="5" t="n">
         <f aca="false" t="array" ref="J26:J26">_xlfn.IFS(AND($I26&gt;=$M$6,$I26&lt;$M$7),$N$6,AND($I26&gt;=$M$7,$I26&lt;$M$8),$N$7,$I26&gt;=$M$8,$N$8+($I26-$M$8)/5)</f>
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="K26" s="5"/>
-      <c r="M26" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="N26" s="5" t="n">
-        <f aca="false" t="array" ref="N26:N26">_xlfn.IFS(AND($M26&gt;=$M$6,$M26&lt;$M$7),$N$6,AND($M26&gt;=$M$7,$M26&lt;$M$8),$N$7,$M26&gt;=$M$8,$N$8+($M26-$M$8)/5)</f>
-        <v>310</v>
-      </c>
-      <c r="O26" s="0" t="n">
-        <f aca="false">ROUNDDOWN(N26/E26,0)</f>
-        <v>51</v>
-      </c>
-      <c r="P26" s="0" t="n">
-        <f aca="false">MIN((ROUNDDOWN(N26,0)),ROUNDDOWN(((((M26)/1000)*80)-(60*(D26/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q26" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P26/2,0)</f>
-        <v>67</v>
-      </c>
+      <c r="M26" s="9"/>
+      <c r="N26" s="5"/>
       <c r="R26" s="11"/>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" s="6" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E27" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F27" s="8" t="n">
-        <f aca="false">200*(D27/1000)+50*((D27/1000)-0.3)*(E27-1)</f>
-        <v>420</v>
-      </c>
-      <c r="G27" s="5" t="n">
-        <f aca="false">ROUNDDOWN(F27/E27,0)</f>
-        <v>70</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I27" s="0" t="n">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="5"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="5"/>
+      <c r="R27" s="11"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="6" t="n">
+        <f aca="false">SUM(G20:G23, J25:J26)-MAX(G20:G23,J25:J26)</f>
+        <v>572</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="6" t="n">
+        <f aca="false">SUM(P20:P23, J25:J26)-MAX(P20:P23,J25:J26)</f>
         <v>850</v>
       </c>
-      <c r="J27" s="5" t="n">
-        <f aca="false" t="array" ref="J27:J27">_xlfn.IFS(AND($I27&gt;=$M$6,$I27&lt;$M$7),$N$6,AND($I27&gt;=$M$7,$I27&lt;$M$8),$N$7,$I27&gt;=$M$8,$N$8+($I27-$M$8)/5)</f>
-        <v>110</v>
-      </c>
-      <c r="K27" s="5"/>
-      <c r="M27" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="N27" s="5" t="n">
-        <f aca="false" t="array" ref="N27:N27">_xlfn.IFS(AND($M27&gt;=$M$6,$M27&lt;$M$7),$N$6,AND($M27&gt;=$M$7,$M27&lt;$M$8),$N$7,$M27&gt;=$M$8,$N$8+($M27-$M$8)/5)</f>
-        <v>310</v>
-      </c>
-      <c r="O27" s="0" t="n">
-        <f aca="false">ROUNDDOWN(N27/E27,0)</f>
-        <v>51</v>
-      </c>
-      <c r="P27" s="0" t="n">
-        <f aca="false">MIN((ROUNDDOWN(N27,0)),ROUNDDOWN(((((M27)/1000)*80)-(60*(D27/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q27" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P27/2,0)</f>
-        <v>67</v>
-      </c>
-      <c r="R27" s="11"/>
-    </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="6" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E28" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F28" s="8" t="n">
-        <f aca="false">200*(D28/1000)+50*((D28/1000)-0.3)*(E28-1)</f>
-        <v>340</v>
-      </c>
-      <c r="G28" s="5" t="n">
-        <f aca="false">ROUNDDOWN(F28/E28,0)</f>
-        <v>85</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I28" s="0" t="n">
-        <v>850</v>
-      </c>
-      <c r="J28" s="5" t="n">
-        <f aca="false" t="array" ref="J28:J28">_xlfn.IFS(AND($I28&gt;=$M$6,$I28&lt;$M$7),$N$6,AND($I28&gt;=$M$7,$I28&lt;$M$8),$N$7,$I28&gt;=$M$8,$N$8+($I28-$M$8)/5)</f>
-        <v>110</v>
-      </c>
-      <c r="K28" s="5"/>
-      <c r="M28" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="N28" s="5" t="n">
-        <f aca="false" t="array" ref="N28:N28">_xlfn.IFS(AND($M28&gt;=$M$6,$M28&lt;$M$7),$N$6,AND($M28&gt;=$M$7,$M28&lt;$M$8),$N$7,$M28&gt;=$M$8,$N$8+($M28-$M$8)/5)</f>
-        <v>310</v>
-      </c>
-      <c r="O28" s="0" t="n">
-        <f aca="false">ROUNDDOWN(N28/E28,0)</f>
-        <v>77</v>
-      </c>
-      <c r="P28" s="0" t="n">
-        <f aca="false">MIN((ROUNDDOWN(N28,0)),ROUNDDOWN((((M28/1000)*80)-(60*(D28/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q28" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P28/2,0)</f>
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="6" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E29" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F29" s="8" t="n">
-        <f aca="false">200*(D29/1000)+50*((D29/1000)-0.3)*(E29-1)</f>
-        <v>340</v>
-      </c>
-      <c r="G29" s="5" t="n">
-        <f aca="false">ROUNDDOWN(F29/E29,0)</f>
-        <v>85</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I29" s="0" t="n">
-        <v>850</v>
-      </c>
-      <c r="J29" s="5" t="n">
-        <f aca="false" t="array" ref="J29:J29">_xlfn.IFS(AND($I29&gt;=$M$6,$I29&lt;$M$7),$N$6,AND($I29&gt;=$M$7,$I29&lt;$M$8),$N$7,$I29&gt;=$M$8,$N$8+($I29-$M$8)/5)</f>
-        <v>110</v>
-      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="M29" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="N29" s="5" t="n">
-        <f aca="false" t="array" ref="N29:N29">_xlfn.IFS(AND($M29&gt;=$M$6,$M29&lt;$M$7),$N$6,AND($M29&gt;=$M$7,$M29&lt;$M$8),$N$7,$M29&gt;=$M$8,$N$8+($M29-$M$8)/5)</f>
-        <v>310</v>
-      </c>
-      <c r="O29" s="0" t="n">
-        <f aca="false">ROUNDDOWN(N29/E29,0)</f>
-        <v>77</v>
-      </c>
-      <c r="P29" s="0" t="n">
-        <f aca="false">MIN((ROUNDDOWN(N29,0)),ROUNDDOWN(((((M29)/1000)*80)-(60*(D29/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q29" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P29/2,0)</f>
-        <v>67</v>
-      </c>
+      <c r="M29" s="9"/>
+      <c r="N29" s="5"/>
       <c r="R29" s="11"/>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="6" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E30" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F30" s="8" t="n">
-        <f aca="false">200*(D30/1000)+50*((D30/1000)-0.3)*(E30-1)</f>
-        <v>340</v>
-      </c>
-      <c r="G30" s="5" t="n">
-        <f aca="false">ROUNDDOWN(F30/E30,0)</f>
-        <v>85</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I30" s="0" t="n">
-        <v>850</v>
-      </c>
-      <c r="J30" s="5" t="n">
-        <f aca="false" t="array" ref="J30:J30">_xlfn.IFS(AND($I30&gt;=$M$6,$I30&lt;$M$7),$N$6,AND($I30&gt;=$M$7,$I30&lt;$M$8),$N$7,$I30&gt;=$M$8,$N$8+($I30-$M$8)/5)</f>
-        <v>110</v>
-      </c>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="J30" s="5"/>
       <c r="K30" s="5"/>
-      <c r="M30" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="N30" s="5" t="n">
-        <f aca="false" t="array" ref="N30:N30">_xlfn.IFS(AND($M30&gt;=$M$6,$M30&lt;$M$7),$N$6,AND($M30&gt;=$M$7,$M30&lt;$M$8),$N$7,$M30&gt;=$M$8,$N$8+($M30-$M$8)/5)</f>
-        <v>310</v>
-      </c>
-      <c r="O30" s="0" t="n">
-        <f aca="false">ROUNDDOWN(N30/E30,0)</f>
-        <v>77</v>
-      </c>
-      <c r="P30" s="0" t="n">
-        <f aca="false">MIN((ROUNDDOWN(N30,0)),ROUNDDOWN(((((M30)/1000)*80)-(60*(D30/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q30" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P30/2,0)</f>
-        <v>67</v>
-      </c>
+      <c r="M30" s="9"/>
+      <c r="N30" s="5"/>
       <c r="R30" s="11"/>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="6" t="n">
-        <v>1100</v>
-      </c>
-      <c r="E31" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F31" s="8" t="n">
-        <f aca="false">200*(D31/1000)+50*((D31/1000)-0.3)*(E31-1)</f>
-        <v>340</v>
-      </c>
-      <c r="G31" s="5" t="n">
-        <f aca="false">ROUNDDOWN(F31/E31,0)</f>
-        <v>85</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I31" s="0" t="n">
-        <v>850</v>
-      </c>
-      <c r="J31" s="5" t="n">
-        <f aca="false" t="array" ref="J31:J31">_xlfn.IFS(AND($I31&gt;=$M$6,$I31&lt;$M$7),$N$6,AND($I31&gt;=$M$7,$I31&lt;$M$8),$N$7,$I31&gt;=$M$8,$N$8+($I31-$M$8)/5)</f>
-        <v>110</v>
-      </c>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="5"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="J31" s="5"/>
       <c r="K31" s="5"/>
-      <c r="M31" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="N31" s="5" t="n">
-        <f aca="false" t="array" ref="N31:N31">_xlfn.IFS(AND($M31&gt;=$M$6,$M31&lt;$M$7),$N$6,AND($M31&gt;=$M$7,$M31&lt;$M$8),$N$7,$M31&gt;=$M$8,$N$8+($M31-$M$8)/5)</f>
-        <v>310</v>
-      </c>
-      <c r="O31" s="0" t="n">
-        <f aca="false">ROUNDDOWN(N31/E31,0)</f>
-        <v>77</v>
-      </c>
-      <c r="P31" s="0" t="n">
-        <f aca="false">MIN((ROUNDDOWN(N31,0)),ROUNDDOWN((((M31/1000)*80)-(60*(D31/1000)))*2.5,0))</f>
-        <v>135</v>
-      </c>
-      <c r="Q31" s="0" t="n">
-        <f aca="false">ROUNDDOWN(P31/2,0)</f>
-        <v>67</v>
-      </c>
+      <c r="M31" s="9"/>
+      <c r="N31" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G34" s="1"/>
@@ -3542,15 +3251,15 @@
       </c>
       <c r="C36" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;C$35,$P$20:$P$31)-_xlfn.MAXIFS($P$20:$P$31,$B$20:$B$31,"="&amp;C$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>540</v>
+        <v>630</v>
       </c>
       <c r="D36" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;D$35,$P$20:$P$31)-_xlfn.MAXIFS($P$20:$P$31,$B$20:$B$31,"="&amp;D$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>540</v>
+        <v>0</v>
       </c>
       <c r="E36" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;E$35,$P$20:$P$31)-_xlfn.MAXIFS($P$20:$P$31,$B$20:$B$31,"="&amp;E$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>540</v>
+        <v>0</v>
       </c>
       <c r="F36" s="14"/>
       <c r="H36" s="14" t="s">
@@ -3576,231 +3285,231 @@
       <c r="B37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="16" t="n">
+      <c r="C37" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;C$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;C$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="D37" s="16" t="n">
+        <v>352</v>
+      </c>
+      <c r="D37" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;D$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;D$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="E37" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;E$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;E$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>340</v>
-      </c>
-      <c r="M37" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M37" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="N37" s="18" t="n">
+      <c r="N37" s="17" t="n">
         <v>3300</v>
       </c>
-      <c r="O37" s="18" t="n">
+      <c r="O37" s="17" t="n">
         <f aca="false">N37/6</f>
         <v>550</v>
       </c>
-      <c r="P37" s="18" t="n">
+      <c r="P37" s="17" t="n">
         <f aca="false">N37/10</f>
         <v>330</v>
       </c>
-      <c r="Q37" s="19" t="n">
+      <c r="Q37" s="18" t="n">
         <f aca="false">N37/SUM(C42:E42)</f>
-        <v>5.89285714285714</v>
+        <v>9.375</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="16" t="n">
+      <c r="C38" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;C$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;C$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="D38" s="16" t="n">
+        <v>352</v>
+      </c>
+      <c r="D38" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;D$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;D$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="E38" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;E$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;E$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>340</v>
-      </c>
-      <c r="M38" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M38" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="N38" s="18" t="n">
+      <c r="N38" s="17" t="n">
         <v>4680</v>
       </c>
-      <c r="O38" s="18" t="n">
+      <c r="O38" s="17" t="n">
         <f aca="false">N38/6</f>
         <v>780</v>
       </c>
-      <c r="P38" s="18" t="n">
+      <c r="P38" s="17" t="n">
         <f aca="false">N38/10</f>
         <v>468</v>
       </c>
-      <c r="Q38" s="19" t="n">
+      <c r="Q38" s="18" t="n">
         <f aca="false">N38/SUM(C41:E41)</f>
-        <v>8.35714285714286</v>
+        <v>13.2954545454545</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="16" t="n">
+      <c r="C39" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;C$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;C$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="D39" s="16" t="n">
+        <v>352</v>
+      </c>
+      <c r="D39" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;D$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;D$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="E39" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;E$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;E$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>340</v>
-      </c>
-      <c r="M39" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="N39" s="18" t="n">
+      <c r="N39" s="17" t="n">
         <v>8060</v>
       </c>
-      <c r="O39" s="18" t="n">
+      <c r="O39" s="17" t="n">
         <f aca="false">N39/6</f>
         <v>1343.33333333333</v>
       </c>
-      <c r="P39" s="18" t="n">
+      <c r="P39" s="17" t="n">
         <f aca="false">N39/10</f>
         <v>806</v>
       </c>
-      <c r="Q39" s="19" t="n">
+      <c r="Q39" s="18" t="n">
         <f aca="false">N39/SUM(C40:E40)</f>
-        <v>8.95555555555556</v>
+        <v>22.8977272727273</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="16" t="n">
+      <c r="C40" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;C$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;C$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="D40" s="16" t="n">
+        <v>352</v>
+      </c>
+      <c r="D40" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;D$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;D$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="E40" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;E$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;E$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>340</v>
-      </c>
-      <c r="M40" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="N40" s="18" t="n">
+      <c r="N40" s="17" t="n">
         <v>8060</v>
       </c>
-      <c r="O40" s="18" t="n">
+      <c r="O40" s="17" t="n">
         <f aca="false">N40/6</f>
         <v>1343.33333333333</v>
       </c>
-      <c r="P40" s="18" t="n">
+      <c r="P40" s="17" t="n">
         <f aca="false">N40/10</f>
         <v>806</v>
       </c>
-      <c r="Q40" s="19" t="n">
+      <c r="Q40" s="18" t="n">
         <f aca="false">N40/SUM(C39:E39)</f>
-        <v>8.95555555555556</v>
+        <v>22.8977272727273</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="16" t="n">
+      <c r="C41" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;C$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;C$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="D41" s="16" t="n">
+        <v>352</v>
+      </c>
+      <c r="D41" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;D$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;D$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="E41" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="M41" s="17" t="n">
+      <c r="M41" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="N41" s="18" t="n">
+      <c r="N41" s="17" t="n">
         <v>8060</v>
       </c>
-      <c r="O41" s="18" t="n">
+      <c r="O41" s="17" t="n">
         <f aca="false">N41/6</f>
         <v>1343.33333333333</v>
       </c>
-      <c r="P41" s="18" t="n">
+      <c r="P41" s="17" t="n">
         <f aca="false">N41/10</f>
         <v>806</v>
       </c>
-      <c r="Q41" s="19" t="n">
+      <c r="Q41" s="18" t="n">
         <f aca="false">N41/SUM(C38:E38)</f>
-        <v>8.95555555555556</v>
+        <v>22.8977272727273</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="16" t="n">
+      <c r="C42" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;C$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;C$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="D42" s="16" t="n">
+        <v>352</v>
+      </c>
+      <c r="D42" s="13" t="n">
         <f aca="false">SUMIF($B$20:$B$31,"="&amp;D$35,$G$20:$G$31)-_xlfn.MAXIFS($G$20:$G$31,$B$20:$B$31,"="&amp;D$35,$H$20:$H$31,"="&amp;"No")</f>
-        <v>280</v>
-      </c>
-      <c r="E42" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="M42" s="17" t="n">
+      <c r="M42" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="N42" s="18" t="n">
+      <c r="N42" s="17" t="n">
         <v>7960</v>
       </c>
-      <c r="O42" s="18" t="n">
+      <c r="O42" s="17" t="n">
         <f aca="false">N42/6</f>
         <v>1326.66666666667</v>
       </c>
-      <c r="P42" s="18" t="n">
+      <c r="P42" s="17" t="n">
         <f aca="false">N42/10</f>
         <v>796</v>
       </c>
-      <c r="Q42" s="19" t="n">
+      <c r="Q42" s="18" t="n">
         <f aca="false">N42/SUM(C37:E37)</f>
-        <v>8.84444444444445</v>
+        <v>22.6136363636364</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="M43" s="17" t="s">
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="M43" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="N43" s="18" t="n">
+      <c r="N43" s="17" t="n">
         <v>7380</v>
       </c>
-      <c r="O43" s="18" t="n">
+      <c r="O43" s="17" t="n">
         <f aca="false">N43/6</f>
         <v>1230</v>
       </c>
-      <c r="P43" s="18" t="n">
+      <c r="P43" s="17" t="n">
         <f aca="false">N43/10</f>
         <v>738</v>
       </c>
-      <c r="Q43" s="19" t="n">
+      <c r="Q43" s="18" t="n">
         <f aca="false">N43/SUM(C36:E36)</f>
-        <v>4.55555555555556</v>
+        <v>11.7142857142857</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3809,44 +3518,44 @@
       </c>
       <c r="C44" s="12" t="n">
         <f aca="false">SUM(C36:C42)</f>
-        <v>2220</v>
+        <v>2742</v>
       </c>
       <c r="D44" s="12" t="n">
         <f aca="false">SUM(D36:D42)</f>
-        <v>2220</v>
+        <v>0</v>
       </c>
       <c r="E44" s="12" t="n">
         <f aca="false">SUM(E36:E42)</f>
-        <v>1900</v>
+        <v>0</v>
       </c>
       <c r="G44" s="1"/>
-      <c r="M44" s="17" t="s">
+      <c r="M44" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="N44" s="18" t="n">
+      <c r="N44" s="17" t="n">
         <f aca="false">SUM(N37:N43)</f>
         <v>47500</v>
       </c>
-      <c r="O44" s="18" t="n">
+      <c r="O44" s="17" t="n">
         <f aca="false">SUM(O37:O43)</f>
         <v>7916.66666666667</v>
       </c>
-      <c r="P44" s="18" t="n">
+      <c r="P44" s="17" t="n">
         <f aca="false">SUM(P37:P43)</f>
         <v>4750</v>
       </c>
-      <c r="Q44" s="19" t="e">
+      <c r="Q44" s="18" t="e">
         <f aca="false">N44/SUM(C49:E49)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="20" t="n">
+      <c r="C45" s="19" t="n">
         <f aca="false">SUM(C44:E44)</f>
-        <v>6340</v>
-      </c>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
+        <v>2742</v>
+      </c>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>